<commit_message>
Additional run data for the beam
</commit_message>
<xml_diff>
--- a/data/runsMarch/InterpolatedResults.xlsx
+++ b/data/runsMarch/InterpolatedResults.xlsx
@@ -82,7 +82,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H122"/>
+  <dimension ref="A1:H145"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2206,1067 +2206,1665 @@
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.00038182392884372258</v>
+        <v>0.00038190702555164122</v>
       </c>
       <c r="B82" s="0">
-        <v>0.00035403039842678725</v>
+        <v>0.00024187628176720568</v>
       </c>
       <c r="C82" s="0">
-        <v>0.00029786839697544439</v>
+        <v>0.00016512370573654558</v>
       </c>
       <c r="D82" s="0">
-        <v>0.00028047487531956641</v>
+        <v>0.00029450076410619715</v>
       </c>
       <c r="E82" s="0">
-        <v>0.00015149541401110123</v>
+        <v>0.00016332899664804379</v>
       </c>
       <c r="F82" s="0">
-        <v>7.3537178411631562e-05</v>
+        <v>0.00012439724561548262</v>
       </c>
       <c r="G82" s="0">
-        <v>4.7948218254677212e-05</v>
+        <v>4.9228100637562747e-05</v>
       </c>
       <c r="H82" s="0">
-        <v>18</v>
+        <v>8.0999999999999996</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>0.00042263658554286913</v>
+        <v>0.00045925821360923906</v>
       </c>
       <c r="B83" s="0">
-        <v>0.00039022460742583592</v>
+        <v>0.00025523360670618063</v>
       </c>
       <c r="C83" s="0">
-        <v>0.0002824991476365973</v>
+        <v>0.00017475506265001966</v>
       </c>
       <c r="D83" s="0">
-        <v>0.00025123454853737641</v>
+        <v>0.00023197645399472439</v>
       </c>
       <c r="E83" s="0">
-        <v>0.00015649654231147101</v>
+        <v>0.00015877231096462618</v>
       </c>
       <c r="F83" s="0">
-        <v>8.6109326009228211e-05</v>
+        <v>0.00015319431508503206</v>
       </c>
       <c r="G83" s="0">
-        <v>4.4668336411425145e-05</v>
+        <v>4.771167298057422e-05</v>
       </c>
       <c r="H83" s="0">
-        <v>18.100000000000001</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>0.00038507274854935063</v>
+        <v>0.00040022119454237486</v>
       </c>
       <c r="B84" s="0">
-        <v>0.00036483926768487594</v>
+        <v>0.00029830481095851751</v>
       </c>
       <c r="C84" s="0">
-        <v>0.00031992875715390091</v>
+        <v>0.00015134677860290427</v>
       </c>
       <c r="D84" s="0">
-        <v>0.00026506155257288694</v>
+        <v>0.00022872783642040003</v>
       </c>
       <c r="E84" s="0">
-        <v>0.0001591575848330936</v>
+        <v>0.00017867062252951751</v>
       </c>
       <c r="F84" s="0">
-        <v>9.78150678888276e-05</v>
+        <v>0.00012621813961949808</v>
       </c>
       <c r="G84" s="0">
-        <v>4.9136529576521611e-05</v>
+        <v>4.8063287284686028e-05</v>
       </c>
       <c r="H84" s="0">
-        <v>18.199999999999999</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.0004327808641336705</v>
+        <v>0.00040383808524588208</v>
       </c>
       <c r="B85" s="0">
-        <v>0.0003758961980946703</v>
+        <v>0.0002504314340632173</v>
       </c>
       <c r="C85" s="0">
-        <v>0.00028380656905634393</v>
+        <v>0.00013600515401163729</v>
       </c>
       <c r="D85" s="0">
-        <v>0.00026968978035771517</v>
+        <v>0.00022536510869465993</v>
       </c>
       <c r="E85" s="0">
-        <v>0.00015331144650088585</v>
+        <v>0.00016342468793415827</v>
       </c>
       <c r="F85" s="0">
-        <v>0.0001087361715420914</v>
+        <v>0.00014209258435510699</v>
       </c>
       <c r="G85" s="0">
-        <v>4.3458412126515643e-05</v>
+        <v>4.7867808315479608e-05</v>
       </c>
       <c r="H85" s="0">
-        <v>18.300000000000001</v>
+        <v>8.4000000000000004</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>0.00038938738530532144</v>
+        <v>0.00042171128960567171</v>
       </c>
       <c r="B86" s="0">
-        <v>0.00037742531329545569</v>
+        <v>0.00029227004169309051</v>
       </c>
       <c r="C86" s="0">
-        <v>0.00036146000000000003</v>
+        <v>0.00010390248534832461</v>
       </c>
       <c r="D86" s="0">
-        <v>0.00025353881884849821</v>
+        <v>0.00022289410199403421</v>
       </c>
       <c r="E86" s="0">
-        <v>0.000169765067159418</v>
+        <v>0.00017064304297877852</v>
       </c>
       <c r="F86" s="0">
-        <v>9.6568531907344939e-05</v>
+        <v>0.00012960475569912945</v>
       </c>
       <c r="G86" s="0">
-        <v>5.1150164233478986e-05</v>
+        <v>4.781413833124634e-05</v>
       </c>
       <c r="H86" s="0">
-        <v>18.399999999999999</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>0.00044421328440124344</v>
+        <v>0.00038198483981036755</v>
       </c>
       <c r="B87" s="0">
-        <v>0.0003642544185057215</v>
+        <v>0.00026242984295053653</v>
       </c>
       <c r="C87" s="0">
-        <v>0.00028782486224797951</v>
+        <v>8.9713910473169541e-05</v>
       </c>
       <c r="D87" s="0">
-        <v>0.00030739999999999999</v>
+        <v>0.00022648424785409423</v>
       </c>
       <c r="E87" s="0">
-        <v>0.0001540231045654136</v>
+        <v>0.0001743033785486893</v>
       </c>
       <c r="F87" s="0">
-        <v>0.00010757903629168223</v>
+        <v>0.00013619673386418871</v>
       </c>
       <c r="G87" s="0">
-        <v>4.2544425759221937e-05</v>
+        <v>4.8080926577691378e-05</v>
       </c>
       <c r="H87" s="0">
-        <v>18.5</v>
+        <v>8.5999999999999996</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.000395478019881029</v>
+        <v>0.00038128223001556718</v>
       </c>
       <c r="B88" s="0">
-        <v>0.00039237312034107684</v>
+        <v>0.00027182848397163902</v>
       </c>
       <c r="C88" s="0">
-        <v>0.00032062359078040476</v>
+        <v>6.7011026494645846e-05</v>
       </c>
       <c r="D88" s="0">
-        <v>0.00024596695212480594</v>
+        <v>0.0002254789491314943</v>
       </c>
       <c r="E88" s="0">
-        <v>0.00018491724810573763</v>
+        <v>0.00016456017709918548</v>
       </c>
       <c r="F88" s="0">
-        <v>9.6163265471782165e-05</v>
+        <v>0.00013374545468755532</v>
       </c>
       <c r="G88" s="0">
-        <v>5.2483345942018852e-05</v>
+        <v>4.7620783167859545e-05</v>
       </c>
       <c r="H88" s="0">
-        <v>18.600000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>0.00037988763299700456</v>
+        <v>0.00037621966581195072</v>
       </c>
       <c r="B89" s="0">
-        <v>0.00033764902196670046</v>
+        <v>0.00028239841630387533</v>
       </c>
       <c r="C89" s="0">
-        <v>0.0002831291216530299</v>
+        <v>4.5532254725703601e-05</v>
       </c>
       <c r="D89" s="0">
-        <v>0.00028825940875697485</v>
+        <v>0.00023224427713454209</v>
       </c>
       <c r="E89" s="0">
-        <v>0.00016141810289328301</v>
+        <v>0.00020032000000000001</v>
       </c>
       <c r="F89" s="0">
-        <v>0.00010083520724207844</v>
+        <v>0.00013101713165392508</v>
       </c>
       <c r="G89" s="0">
-        <v>4.1923998804146153e-05</v>
+        <v>4.8348960310011766e-05</v>
       </c>
       <c r="H89" s="0">
-        <v>18.699999999999999</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>0.00040208612668883972</v>
+        <v>0.00040343330039332856</v>
       </c>
       <c r="B90" s="0">
-        <v>0.00042482068432186606</v>
+        <v>0.00029924810213660837</v>
       </c>
       <c r="C90" s="0">
-        <v>0.00029889649533664599</v>
+        <v>2.9954305994424126e-05</v>
       </c>
       <c r="D90" s="0">
-        <v>0.00024201213489089728</v>
+        <v>0.00024787985007119844</v>
       </c>
       <c r="E90" s="0">
-        <v>0.00018675160468337106</v>
+        <v>0.00016047880814756336</v>
       </c>
       <c r="F90" s="0">
-        <v>0.00010102874000619502</v>
+        <v>0.000138806908929089</v>
       </c>
       <c r="G90" s="0">
-        <v>4.6006869579689803e-05</v>
+        <v>4.7555520991042443e-05</v>
       </c>
       <c r="H90" s="0">
-        <v>18.800000000000001</v>
+        <v>8.9000000000000004</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.00037988915471760571</v>
+        <v>0.00037900669276909934</v>
       </c>
       <c r="B91" s="0">
-        <v>0.00034450036034599114</v>
+        <v>0.00030912368370980607</v>
       </c>
       <c r="C91" s="0">
-        <v>0.00028649627340217283</v>
+        <v>1.0850986591972306e-05</v>
       </c>
       <c r="D91" s="0">
-        <v>0.00030737098996192326</v>
+        <v>0.00024357026291995184</v>
       </c>
       <c r="E91" s="0">
-        <v>0.00015511119957767403</v>
+        <v>0.00017426329750029197</v>
       </c>
       <c r="F91" s="0">
-        <v>0.00010359665977772487</v>
+        <v>0.00012680915564372959</v>
       </c>
       <c r="G91" s="0">
-        <v>4.161672214846615e-05</v>
+        <v>4.8778864438036099e-05</v>
       </c>
       <c r="H91" s="0">
-        <v>18.899999999999999</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0">
-        <v>0.00040953265912630729</v>
+        <v>0.00045381990010178635</v>
       </c>
       <c r="B92" s="0">
-        <v>0.00042463236636216303</v>
+        <v>0.00036452329892419855</v>
       </c>
       <c r="C92" s="0">
-        <v>0.00028788027265744584</v>
+        <v>4.7170541738531805e-06</v>
       </c>
       <c r="D92" s="0">
-        <v>0.00024149277651625922</v>
+        <v>0.00022913118522265182</v>
       </c>
       <c r="E92" s="0">
-        <v>0.0001736803913727378</v>
+        <v>0.00015810849884878336</v>
       </c>
       <c r="F92" s="0">
-        <v>0.00010850719496213222</v>
+        <v>0.00014625765616968679</v>
       </c>
       <c r="G92" s="0">
-        <v>4.1706947000387257e-05</v>
+        <v>4.7595018554241687e-05</v>
       </c>
       <c r="H92" s="0">
-        <v>19</v>
+        <v>9.0999999999999996</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>0.00038151463633301439</v>
+        <v>0.00038722868839452036</v>
       </c>
       <c r="B93" s="0">
-        <v>0.00035289061045873989</v>
+        <v>0.00034032323867337302</v>
       </c>
       <c r="C93" s="0">
-        <v>0.00029604826280225845</v>
+        <v>5.3280999999999999e-06</v>
       </c>
       <c r="D93" s="0">
-        <v>0.00028235815716253578</v>
+        <v>0.00025163492643683294</v>
       </c>
       <c r="E93" s="0">
-        <v>0.00015589537214092853</v>
+        <v>0.00016255143418323565</v>
       </c>
       <c r="F93" s="0">
-        <v>0.00011065198203045973</v>
+        <v>0.0001240765467755187</v>
       </c>
       <c r="G93" s="0">
-        <v>4.132260987058966e-05</v>
+        <v>4.9341120663629527e-05</v>
       </c>
       <c r="H93" s="0">
-        <v>19.100000000000001</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>0.0004177687477483571</v>
+        <v>0.00044213585309491705</v>
       </c>
       <c r="B94" s="0">
-        <v>0.00039832923599365545</v>
+        <v>0.00032991060457048682</v>
       </c>
       <c r="C94" s="0">
-        <v>0.00028320127519340432</v>
+        <v>2.504825414403166e-05</v>
       </c>
       <c r="D94" s="0">
-        <v>0.0002458344506389971</v>
+        <v>0.00019680789807607346</v>
       </c>
       <c r="E94" s="0">
-        <v>0.00016401626080857697</v>
+        <v>0.00015818677239704578</v>
       </c>
       <c r="F94" s="0">
-        <v>0.00011891532946045304</v>
+        <v>0.00015333061500574373</v>
       </c>
       <c r="G94" s="0">
-        <v>3.7914432128473924e-05</v>
+        <v>4.7716143016695487e-05</v>
       </c>
       <c r="H94" s="0">
-        <v>19.199999999999999</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0">
-        <v>0.0003843650390263374</v>
+        <v>0.00040046265928052392</v>
       </c>
       <c r="B95" s="0">
-        <v>0.00036279192915659179</v>
+        <v>0.00039355897503198935</v>
       </c>
       <c r="C95" s="0">
-        <v>0.00031505567726572263</v>
+        <v>4.6214528581696345e-05</v>
       </c>
       <c r="D95" s="0">
-        <v>0.00026760875237498725</v>
+        <v>0.00020645206875936637</v>
       </c>
       <c r="E95" s="0">
-        <v>0.00016127307586172047</v>
+        <v>0.00015809931002950644</v>
       </c>
       <c r="F95" s="0">
-        <v>0.00012749704438623597</v>
+        <v>0.00012214466812889891</v>
       </c>
       <c r="G95" s="0">
-        <v>4.122909806432214e-05</v>
+        <v>4.9803702523135962e-05</v>
       </c>
       <c r="H95" s="0">
-        <v>19.300000000000001</v>
+        <v>9.4000000000000004</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>0.00042698230145499152</v>
+        <v>0.0004019802467837766</v>
       </c>
       <c r="B96" s="0">
-        <v>0.00038360380828790546</v>
+        <v>0.00031265103656252932</v>
       </c>
       <c r="C96" s="0">
-        <v>0.00028267210479419847</v>
+        <v>6.875637210751081e-05</v>
       </c>
       <c r="D96" s="0">
-        <v>0.00025786451662419764</v>
+        <v>0.00017997133249208089</v>
       </c>
       <c r="E96" s="0">
-        <v>0.00015857461803323489</v>
+        <v>0.00016180345080185469</v>
       </c>
       <c r="F96" s="0">
-        <v>0.00013106221553029531</v>
+        <v>0.00014311235959896514</v>
       </c>
       <c r="G96" s="0">
-        <v>3.4659511520834067e-05</v>
+        <v>4.7867639685149564e-05</v>
       </c>
       <c r="H96" s="0">
-        <v>19.399999999999999</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>0.00038824260111763263</v>
+        <v>0.00041658542741644135</v>
       </c>
       <c r="B97" s="0">
-        <v>0.00037412402798497554</v>
+        <v>0.00037527708774465668</v>
       </c>
       <c r="C97" s="0">
-        <v>0.00034913908421271633</v>
+        <v>8.4392630078950089e-05</v>
       </c>
       <c r="D97" s="0">
-        <v>0.00025563690795786422</v>
+        <v>0.00017208274099342726</v>
       </c>
       <c r="E97" s="0">
-        <v>0.00017032375255516448</v>
+        <v>0.00017489644723101244</v>
       </c>
       <c r="F97" s="0">
-        <v>0.0001269646056787803</v>
+        <v>0.00012761087791473804</v>
       </c>
       <c r="G97" s="0">
-        <v>4.1314984616979181e-05</v>
+        <v>4.7955750930324525e-05</v>
       </c>
       <c r="H97" s="0">
-        <v>19.5</v>
+        <v>9.5999999999999996</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0">
-        <v>0.00043689789063666772</v>
+        <v>0.0003846316800709739</v>
       </c>
       <c r="B98" s="0">
-        <v>0.00037119469745727378</v>
+        <v>0.0003137616719615962</v>
       </c>
       <c r="C98" s="0">
-        <v>0.00028499719891668499</v>
+        <v>0.00010708815323919967</v>
       </c>
       <c r="D98" s="0">
-        <v>0.00027943614250291402</v>
+        <v>0.00016870401926936642</v>
       </c>
       <c r="E98" s="0">
-        <v>0.00015604071960330259</v>
+        <v>0.00017420242592938709</v>
       </c>
       <c r="F98" s="0">
-        <v>0.00014391932939816443</v>
+        <v>0.00013636271703758031</v>
       </c>
       <c r="G98" s="0">
-        <v>3.1747541055753856e-05</v>
+        <v>4.8076943927806698e-05</v>
       </c>
       <c r="H98" s="0">
-        <v>19.600000000000001</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>0.00039302186621724362</v>
+        <v>0.00043608442075998978</v>
       </c>
       <c r="B99" s="0">
-        <v>0.00038760809623591323</v>
+        <v>0.00035458273549404234</v>
       </c>
       <c r="C99" s="0">
-        <v>0.00032998932637252844</v>
+        <v>0.0001201412357804995</v>
       </c>
       <c r="D99" s="0">
-        <v>0.0002479592542960384</v>
+        <v>0.00015706803303272413</v>
       </c>
       <c r="E99" s="0">
-        <v>0.00018223999991138663</v>
+        <v>0.00016746061239393076</v>
       </c>
       <c r="F99" s="0">
-        <v>0.00011671766886766412</v>
+        <v>0.00013179825727761572</v>
       </c>
       <c r="G99" s="0">
-        <v>3.3955822806207834e-05</v>
+        <v>4.773682409243373e-05</v>
       </c>
       <c r="H99" s="0">
-        <v>19.699999999999999</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>0.00037983548707013382</v>
+        <v>0.00037923017198348853</v>
       </c>
       <c r="B100" s="0">
-        <v>0.00033760889927089862</v>
+        <v>0.00032398410528741901</v>
       </c>
       <c r="C100" s="0">
-        <v>0.00028311314861404206</v>
+        <v>0.00013757732382510822</v>
       </c>
       <c r="D100" s="0">
-        <v>0.0002882853969048376</v>
+        <v>0.00015662267873007711</v>
       </c>
       <c r="E100" s="0">
-        <v>0.00016347221474073315</v>
+        <v>0.00020019999999999999</v>
       </c>
       <c r="F100" s="0">
-        <v>0.00011742811815592588</v>
+        <v>0.00013104099418396415</v>
       </c>
       <c r="G100" s="0">
-        <v>2.8937451254732675e-05</v>
+        <v>4.8340533105155304e-05</v>
       </c>
       <c r="H100" s="0">
-        <v>19.800000000000001</v>
+        <v>9.9000000000000004</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0">
-        <v>0.00039958924597638374</v>
+        <v>0.00042638276419349169</v>
       </c>
       <c r="B101" s="0">
-        <v>0.00040377288248296436</v>
+        <v>0.00035853563356245775</v>
       </c>
       <c r="C101" s="0">
-        <v>0.00030492034402949817</v>
+        <v>0.00016896357128347073</v>
       </c>
       <c r="D101" s="0">
-        <v>0.00024303134599600778</v>
+        <v>0.00014774597068114878</v>
       </c>
       <c r="E101" s="0">
-        <v>0.00019827081250733467</v>
+        <v>0.00016178444363739518</v>
       </c>
       <c r="F101" s="0">
-        <v>0.00011545632363013652</v>
+        <v>0.00013655923662258537</v>
       </c>
       <c r="G101" s="0">
-        <v>2.7963381969978955e-05</v>
+        <v>4.7614872068611207e-05</v>
       </c>
       <c r="H101" s="0">
-        <v>19.899999999999999</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>0.00037983098980074289</v>
+        <v>0.00038082784677543539</v>
       </c>
       <c r="B102" s="0">
-        <v>0.00034398992418763235</v>
+        <v>0.00034118031381534628</v>
       </c>
       <c r="C102" s="0">
-        <v>0.00028608230498257907</v>
+        <v>0.00017163702083430215</v>
       </c>
       <c r="D102" s="0">
-        <v>0.0003074004775742926</v>
+        <v>0.00014529751719807144</v>
       </c>
       <c r="E102" s="0">
-        <v>0.00015706290094026192</v>
+        <v>0.00017228365410193217</v>
       </c>
       <c r="F102" s="0">
-        <v>0.0001163716197775485</v>
+        <v>0.00012670721766910384</v>
       </c>
       <c r="G102" s="0">
-        <v>2.5848217007533918e-05</v>
+        <v>4.8766321253744418e-05</v>
       </c>
       <c r="H102" s="0">
-        <v>20</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>0.0004063478779601894</v>
+        <v>0.00048968000000000004</v>
       </c>
       <c r="B103" s="0">
-        <v>0.00042464983324247402</v>
+        <v>0.00038867981041557076</v>
       </c>
       <c r="C103" s="0">
-        <v>0.00029142654136816136</v>
+        <v>0.00022564918100123111</v>
       </c>
       <c r="D103" s="0">
-        <v>0.00024125164485324738</v>
+        <v>0.00013215526488212831</v>
       </c>
       <c r="E103" s="0">
-        <v>0.00018026720262323309</v>
+        <v>0.00015820938036765087</v>
       </c>
       <c r="F103" s="0">
-        <v>0.00011845174607069648</v>
+        <v>0.00014317965570007996</v>
       </c>
       <c r="G103" s="0">
-        <v>2.275058031244153e-05</v>
+        <v>4.757753291123527e-05</v>
       </c>
       <c r="H103" s="0">
-        <v>20.100000000000001</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0">
-        <v>0.00038120676550941756</v>
+        <v>0.00038698720232883477</v>
       </c>
       <c r="B104" s="0">
-        <v>0.00035179326377914581</v>
+        <v>0.00036316966388530192</v>
       </c>
       <c r="C104" s="0">
-        <v>0.00029452938714597578</v>
+        <v>0.00022601324309436059</v>
       </c>
       <c r="D104" s="0">
-        <v>0.00028425145520624473</v>
+        <v>0.00011816209262457394</v>
       </c>
       <c r="E104" s="0">
-        <v>0.00015697971490512307</v>
+        <v>0.00016062120117911954</v>
       </c>
       <c r="F104" s="0">
-        <v>0.00011984659736553046</v>
+        <v>0.00012374222065109994</v>
       </c>
       <c r="G104" s="0">
-        <v>2.2644821219429934e-05</v>
+        <v>4.9367281694106745e-05</v>
       </c>
       <c r="H104" s="0">
-        <v>20.199999999999999</v>
+        <v>10.300000000000001</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>0.00041378708156663299</v>
+        <v>0.00038182392884372258</v>
       </c>
       <c r="B105" s="0">
-        <v>0.00042448463195362987</v>
+        <v>0.00035403039842678725</v>
       </c>
       <c r="C105" s="0">
-        <v>0.00028473478194058718</v>
+        <v>0.00029786839697544439</v>
       </c>
       <c r="D105" s="0">
-        <v>0.00024319064967143702</v>
+        <v>0.00028047487531956641</v>
       </c>
       <c r="E105" s="0">
-        <v>0.00016929372878680523</v>
+        <v>0.00015149541401110123</v>
       </c>
       <c r="F105" s="0">
-        <v>0.00012460069601209908</v>
+        <v>7.3537178411631562e-05</v>
       </c>
       <c r="G105" s="0">
-        <v>1.824228755658202e-05</v>
+        <v>4.7948218254677212e-05</v>
       </c>
       <c r="H105" s="0">
-        <v>20.300000000000001</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>0.00038376282909770846</v>
+        <v>0.00042263658554286913</v>
       </c>
       <c r="B106" s="0">
-        <v>0.00036097595321465877</v>
+        <v>0.00039022460742583592</v>
       </c>
       <c r="C106" s="0">
-        <v>0.00031096640651309617</v>
+        <v>0.0002824991476365973</v>
       </c>
       <c r="D106" s="0">
-        <v>0.00026928131260034178</v>
+        <v>0.00025123454853737641</v>
       </c>
       <c r="E106" s="0">
-        <v>0.00016104794860451703</v>
+        <v>0.00015649654231147101</v>
       </c>
       <c r="F106" s="0">
-        <v>0.00013288495477084623</v>
+        <v>8.6109326009228211e-05</v>
       </c>
       <c r="G106" s="0">
-        <v>1.9347511244878296e-05</v>
+        <v>4.4668336411425145e-05</v>
       </c>
       <c r="H106" s="0">
-        <v>20.399999999999999</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0">
-        <v>0.00042187544335182264</v>
+        <v>0.00038507274854935063</v>
       </c>
       <c r="B107" s="0">
-        <v>0.00039093559282772172</v>
+        <v>0.00036483926768487594</v>
       </c>
       <c r="C107" s="0">
-        <v>0.00028252524279334733</v>
+        <v>0.00031992875715390091</v>
       </c>
       <c r="D107" s="0">
-        <v>0.00024999799529348176</v>
+        <v>0.00026506155257288694</v>
       </c>
       <c r="E107" s="0">
-        <v>0.0001621066211818428</v>
+        <v>0.0001591575848330936</v>
       </c>
       <c r="F107" s="0">
-        <v>0.00013308714892742643</v>
+        <v>9.78150678888276e-05</v>
       </c>
       <c r="G107" s="0">
-        <v>1.5003134306951252e-05</v>
+        <v>4.9136529576521611e-05</v>
       </c>
       <c r="H107" s="0">
-        <v>20.5</v>
+        <v>18.199999999999999</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>0.0003871828654738752</v>
+        <v>0.0004327808641336705</v>
       </c>
       <c r="B108" s="0">
-        <v>0.00037154372527705153</v>
+        <v>0.0003758961980946703</v>
       </c>
       <c r="C108" s="0">
-        <v>0.0003396030549550627</v>
+        <v>0.00028380656905634393</v>
       </c>
       <c r="D108" s="0">
-        <v>0.00025781872525527998</v>
+        <v>0.00026968978035771517</v>
       </c>
       <c r="E108" s="0">
-        <v>0.0001688210294553972</v>
+        <v>0.00015331144650088585</v>
       </c>
       <c r="F108" s="0">
-        <v>0.00013846482500039895</v>
+        <v>0.0001087361715420914</v>
       </c>
       <c r="G108" s="0">
-        <v>1.2002590161856953e-05</v>
+        <v>4.3458412126515643e-05</v>
       </c>
       <c r="H108" s="0">
-        <v>20.600000000000001</v>
+        <v>18.300000000000001</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>0.00043085233765042716</v>
+        <v>0.00038938738530532144</v>
       </c>
       <c r="B109" s="0">
-        <v>0.00037819065336362794</v>
+        <v>0.00037742531329545569</v>
       </c>
       <c r="C109" s="0">
-        <v>0.00028332445968963456</v>
+        <v>0.00036146000000000003</v>
       </c>
       <c r="D109" s="0">
-        <v>0.00026436500717624698</v>
+        <v>0.00025353881884849821</v>
       </c>
       <c r="E109" s="0">
-        <v>0.00015797161384160775</v>
+        <v>0.000169765067159418</v>
       </c>
       <c r="F109" s="0">
-        <v>0.00015034149727199568</v>
+        <v>9.6568531907344939e-05</v>
       </c>
       <c r="G109" s="0">
-        <v>8.5612956049812498e-06</v>
+        <v>5.1150164233478986e-05</v>
       </c>
       <c r="H109" s="0">
-        <v>20.699999999999999</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0">
-        <v>0.00039149361122131447</v>
+        <v>0.00044421328440124344</v>
       </c>
       <c r="B110" s="0">
-        <v>0.00038359245943870484</v>
+        <v>0.0003642544185057215</v>
       </c>
       <c r="C110" s="0">
-        <v>0.00034011643811539868</v>
+        <v>0.00028782486224797951</v>
       </c>
       <c r="D110" s="0">
-        <v>0.00024986016418736306</v>
+        <v>0.00030739999999999999</v>
       </c>
       <c r="E110" s="0">
-        <v>0.0001795921596561774</v>
+        <v>0.0001540231045654136</v>
       </c>
       <c r="F110" s="0">
-        <v>0.00012304716506929478</v>
+        <v>0.00010757903629168223</v>
       </c>
       <c r="G110" s="0">
-        <v>5.9479945467813023e-06</v>
+        <v>4.2544425759221937e-05</v>
       </c>
       <c r="H110" s="0">
-        <v>20.800000000000001</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>0.000440656893928742</v>
+        <v>0.000395478019881029</v>
       </c>
       <c r="B111" s="0">
-        <v>0.00036735654284972887</v>
+        <v>0.00039237312034107684</v>
       </c>
       <c r="C111" s="0">
-        <v>0.0002863404383383508</v>
+        <v>0.00032062359078040476</v>
       </c>
       <c r="D111" s="0">
-        <v>0.00029174097821595135</v>
+        <v>0.00024596695212480594</v>
       </c>
       <c r="E111" s="0">
-        <v>0.00015675414454324827</v>
+        <v>0.00018491724810573763</v>
       </c>
       <c r="F111" s="0">
-        <v>0.00014150962254996257</v>
+        <v>9.6163265471782165e-05</v>
       </c>
       <c r="G111" s="0">
-        <v>3.65434697980964e-06</v>
+        <v>5.2483345942018852e-05</v>
       </c>
       <c r="H111" s="0">
-        <v>20.899999999999999</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>0.00039747572029880909</v>
+        <v>0.00037988763299700456</v>
       </c>
       <c r="B112" s="0">
-        <v>0.00039803527544867643</v>
+        <v>0.00033764902196670046</v>
       </c>
       <c r="C112" s="0">
-        <v>0.00031178624641719452</v>
+        <v>0.0002831291216530299</v>
       </c>
       <c r="D112" s="0">
-        <v>0.00024435826845741994</v>
+        <v>0.00028825940875697485</v>
       </c>
       <c r="E112" s="0">
-        <v>0.00019891575942469444</v>
+        <v>0.00016141810289328301</v>
       </c>
       <c r="F112" s="0">
-        <v>0.00011915207541288422</v>
+        <v>0.00010083520724207844</v>
       </c>
       <c r="G112" s="0">
-        <v>1.2581511427118601e-06</v>
+        <v>4.1923998804146153e-05</v>
       </c>
       <c r="H112" s="0">
-        <v>21</v>
+        <v>18.699999999999999</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0">
-        <v>0.0003797444405846567</v>
+        <v>0.00040208612668883972</v>
       </c>
       <c r="B113" s="0">
-        <v>0.00034357206672406372</v>
+        <v>0.00042482068432186606</v>
       </c>
       <c r="C113" s="0">
-        <v>0.00028577342983141126</v>
+        <v>0.00029889649533664599</v>
       </c>
       <c r="D113" s="0">
-        <v>0.00030739</v>
+        <v>0.00024201213489089728</v>
       </c>
       <c r="E113" s="0">
-        <v>0.00015743501598607446</v>
+        <v>0.00018675160468337106</v>
       </c>
       <c r="F113" s="0">
-        <v>0.00011956667471726626</v>
+        <v>0.00010102874000619502</v>
       </c>
       <c r="G113" s="0">
-        <v>6.9159639995952087e-07</v>
+        <v>4.6006869579689803e-05</v>
       </c>
       <c r="H113" s="0">
-        <v>21.100000000000001</v>
+        <v>18.800000000000001</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>0.00040361689607648296</v>
+        <v>0.00037988915471760571</v>
       </c>
       <c r="B114" s="0">
-        <v>0.00042464576502440464</v>
+        <v>0.00034450036034599114</v>
       </c>
       <c r="C114" s="0">
-        <v>0.0002956663613593573</v>
+        <v>0.00028649627340217283</v>
       </c>
       <c r="D114" s="0">
-        <v>0.00024159210081356699</v>
+        <v>0.00030737098996192326</v>
       </c>
       <c r="E114" s="0">
-        <v>0.00018544957728718945</v>
+        <v>0.00015511119957767403</v>
       </c>
       <c r="F114" s="0">
-        <v>0.00012018742877616202</v>
+        <v>0.00010359665977772487</v>
       </c>
       <c r="G114" s="0">
-        <v>9.725499999999999e-07</v>
+        <v>4.161672214846615e-05</v>
       </c>
       <c r="H114" s="0">
-        <v>21.199999999999999</v>
+        <v>18.899999999999999</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>0.0003809660629158037</v>
+        <v>0.00040953265912630729</v>
       </c>
       <c r="B115" s="0">
-        <v>0.00035087026423925172</v>
+        <v>0.00042463236636216303</v>
       </c>
       <c r="C115" s="0">
-        <v>0.00029326027649308325</v>
+        <v>0.00028788027265744584</v>
       </c>
       <c r="D115" s="0">
-        <v>0.00028618686855615854</v>
+        <v>0.00024149277651625922</v>
       </c>
       <c r="E115" s="0">
-        <v>0.00015722776997318088</v>
+        <v>0.0001736803913727378</v>
       </c>
       <c r="F115" s="0">
-        <v>0.00012195751661074543</v>
+        <v>0.00010850719496213222</v>
       </c>
       <c r="G115" s="0">
-        <v>4.7116345977890171e-06</v>
+        <v>4.1706947000387257e-05</v>
       </c>
       <c r="H115" s="0">
-        <v>21.300000000000001</v>
+        <v>19</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0">
-        <v>0.00041035747155033239</v>
+        <v>0.00038151463633301439</v>
       </c>
       <c r="B116" s="0">
-        <v>0.00042448388123875755</v>
+        <v>0.00035289061045873989</v>
       </c>
       <c r="C116" s="0">
-        <v>0.00028707223020498163</v>
+        <v>0.00029604826280225845</v>
       </c>
       <c r="D116" s="0">
-        <v>0.00024171529659168208</v>
+        <v>0.00028235815716253578</v>
       </c>
       <c r="E116" s="0">
-        <v>0.00017383658756468307</v>
+        <v>0.00015589537214092853</v>
       </c>
       <c r="F116" s="0">
-        <v>0.00012448773544132324</v>
+        <v>0.00011065198203045973</v>
       </c>
       <c r="G116" s="0">
-        <v>8.430192142771746e-06</v>
+        <v>4.132260987058966e-05</v>
       </c>
       <c r="H116" s="0">
-        <v>21.399999999999999</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>0.00038319494903305099</v>
+        <v>0.0004177687477483571</v>
       </c>
       <c r="B117" s="0">
-        <v>0.0003593751449620789</v>
+        <v>0.00039832923599365545</v>
       </c>
       <c r="C117" s="0">
-        <v>0.00030753489284978986</v>
+        <v>0.00028320127519340432</v>
       </c>
       <c r="D117" s="0">
-        <v>0.00027074786559491768</v>
+        <v>0.0002458344506389971</v>
       </c>
       <c r="E117" s="0">
-        <v>0.00016051914483186972</v>
+        <v>0.00016401626080857697</v>
       </c>
       <c r="F117" s="0">
-        <v>0.00013222268156095837</v>
+        <v>0.00011891532946045304</v>
       </c>
       <c r="G117" s="0">
-        <v>1.2600715313424414e-05</v>
+        <v>3.7914432128473924e-05</v>
       </c>
       <c r="H117" s="0">
-        <v>21.5</v>
+        <v>19.199999999999999</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>0.00041764326938574698</v>
+        <v>0.0003843650390263374</v>
       </c>
       <c r="B118" s="0">
-        <v>0.00039820064724569696</v>
+        <v>0.00036279192915659179</v>
       </c>
       <c r="C118" s="0">
-        <v>0.00028313476522883293</v>
+        <v>0.00031505567726572263</v>
       </c>
       <c r="D118" s="0">
-        <v>0.00024583944851884232</v>
+        <v>0.00026760875237498725</v>
       </c>
       <c r="E118" s="0">
-        <v>0.00016558538425519794</v>
+        <v>0.00016127307586172047</v>
       </c>
       <c r="F118" s="0">
-        <v>0.00013085054366301249</v>
+        <v>0.00012749704438623597</v>
       </c>
       <c r="G118" s="0">
-        <v>1.5168913096303569e-05</v>
+        <v>4.122909806432214e-05</v>
       </c>
       <c r="H118" s="0">
-        <v>21.600000000000001</v>
+        <v>19.300000000000001</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0">
-        <v>0.00038635419994989138</v>
+        <v>0.00042698230145499152</v>
       </c>
       <c r="B119" s="0">
-        <v>0.0003690735522066414</v>
+        <v>0.00038360380828790546</v>
       </c>
       <c r="C119" s="0">
-        <v>0.00033218613670190874</v>
+        <v>0.00028267210479419847</v>
       </c>
       <c r="D119" s="0">
-        <v>0.0002600973316340633</v>
+        <v>0.00025786451662419764</v>
       </c>
       <c r="E119" s="0">
-        <v>0.0001676841002176234</v>
+        <v>0.00015857461803323489</v>
       </c>
       <c r="F119" s="0">
-        <v>0.00014422095733116416</v>
+        <v>0.00013106221553029531</v>
       </c>
       <c r="G119" s="0">
-        <v>1.9473161581188467e-05</v>
+        <v>3.4659511520834067e-05</v>
       </c>
       <c r="H119" s="0">
-        <v>21.699999999999999</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>0.00042570267560940335</v>
+        <v>0.00038824260111763263</v>
       </c>
       <c r="B120" s="0">
-        <v>0.00038497430027418052</v>
+        <v>0.00037412402798497554</v>
       </c>
       <c r="C120" s="0">
-        <v>0.00028249763809656424</v>
+        <v>0.00034913908421271633</v>
       </c>
       <c r="D120" s="0">
-        <v>0.00025600024462552582</v>
+        <v>0.00025563690795786422</v>
       </c>
       <c r="E120" s="0">
-        <v>0.00016021270751400584</v>
+        <v>0.00017032375255516448</v>
       </c>
       <c r="F120" s="0">
-        <v>0.00013980811335005265</v>
+        <v>0.0001269646056787803</v>
       </c>
       <c r="G120" s="0">
-        <v>2.1558839395057611e-05</v>
+        <v>4.1314984616979181e-05</v>
       </c>
       <c r="H120" s="0">
-        <v>21.800000000000001</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>0.00039023478888633022</v>
+        <v>0.00043689789063666772</v>
       </c>
       <c r="B121" s="0">
-        <v>0.00038020383533981958</v>
+        <v>0.00037119469745727378</v>
       </c>
       <c r="C121" s="0">
-        <v>0.00035023304669740395</v>
+        <v>0.00028499719891668499</v>
       </c>
       <c r="D121" s="0">
-        <v>0.0002516478799932222</v>
+        <v>0.00027943614250291402</v>
       </c>
       <c r="E121" s="0">
-        <v>0.00017680605361869182</v>
+        <v>0.00015604071960330259</v>
       </c>
       <c r="F121" s="0">
-        <v>0.00012721930476823086</v>
+        <v>0.00014391932939816443</v>
       </c>
       <c r="G121" s="0">
-        <v>2.4767148855892695e-05</v>
+        <v>3.1747541055753856e-05</v>
       </c>
       <c r="H121" s="0">
-        <v>21.899999999999999</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0">
+        <v>0.00039302186621724362</v>
+      </c>
+      <c r="B122" s="0">
+        <v>0.00038760809623591323</v>
+      </c>
+      <c r="C122" s="0">
+        <v>0.00032998932637252844</v>
+      </c>
+      <c r="D122" s="0">
+        <v>0.0002479592542960384</v>
+      </c>
+      <c r="E122" s="0">
+        <v>0.00018223999991138663</v>
+      </c>
+      <c r="F122" s="0">
+        <v>0.00011671766886766412</v>
+      </c>
+      <c r="G122" s="0">
+        <v>3.3955822806207834e-05</v>
+      </c>
+      <c r="H122" s="0">
+        <v>19.699999999999999</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0">
+        <v>0.00037983548707013382</v>
+      </c>
+      <c r="B123" s="0">
+        <v>0.00033760889927089862</v>
+      </c>
+      <c r="C123" s="0">
+        <v>0.00028311314861404206</v>
+      </c>
+      <c r="D123" s="0">
+        <v>0.0002882853969048376</v>
+      </c>
+      <c r="E123" s="0">
+        <v>0.00016347221474073315</v>
+      </c>
+      <c r="F123" s="0">
+        <v>0.00011742811815592588</v>
+      </c>
+      <c r="G123" s="0">
+        <v>2.8937451254732675e-05</v>
+      </c>
+      <c r="H123" s="0">
+        <v>19.800000000000001</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0">
+        <v>0.00039958924597638374</v>
+      </c>
+      <c r="B124" s="0">
+        <v>0.00040377288248296436</v>
+      </c>
+      <c r="C124" s="0">
+        <v>0.00030492034402949817</v>
+      </c>
+      <c r="D124" s="0">
+        <v>0.00024303134599600778</v>
+      </c>
+      <c r="E124" s="0">
+        <v>0.00019827081250733467</v>
+      </c>
+      <c r="F124" s="0">
+        <v>0.00011545632363013652</v>
+      </c>
+      <c r="G124" s="0">
+        <v>2.7963381969978955e-05</v>
+      </c>
+      <c r="H124" s="0">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0">
+        <v>0.00037983098980074289</v>
+      </c>
+      <c r="B125" s="0">
+        <v>0.00034398992418763235</v>
+      </c>
+      <c r="C125" s="0">
+        <v>0.00028608230498257907</v>
+      </c>
+      <c r="D125" s="0">
+        <v>0.0003074004775742926</v>
+      </c>
+      <c r="E125" s="0">
+        <v>0.00015706290094026192</v>
+      </c>
+      <c r="F125" s="0">
+        <v>0.0001163716197775485</v>
+      </c>
+      <c r="G125" s="0">
+        <v>2.5848217007533918e-05</v>
+      </c>
+      <c r="H125" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0">
+        <v>0.0004063478779601894</v>
+      </c>
+      <c r="B126" s="0">
+        <v>0.00042464983324247402</v>
+      </c>
+      <c r="C126" s="0">
+        <v>0.00029142654136816136</v>
+      </c>
+      <c r="D126" s="0">
+        <v>0.00024125164485324738</v>
+      </c>
+      <c r="E126" s="0">
+        <v>0.00018026720262323309</v>
+      </c>
+      <c r="F126" s="0">
+        <v>0.00011845174607069648</v>
+      </c>
+      <c r="G126" s="0">
+        <v>2.275058031244153e-05</v>
+      </c>
+      <c r="H126" s="0">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0">
+        <v>0.00038120676550941756</v>
+      </c>
+      <c r="B127" s="0">
+        <v>0.00035179326377914581</v>
+      </c>
+      <c r="C127" s="0">
+        <v>0.00029452938714597578</v>
+      </c>
+      <c r="D127" s="0">
+        <v>0.00028425145520624473</v>
+      </c>
+      <c r="E127" s="0">
+        <v>0.00015697971490512307</v>
+      </c>
+      <c r="F127" s="0">
+        <v>0.00011984659736553046</v>
+      </c>
+      <c r="G127" s="0">
+        <v>2.2644821219429934e-05</v>
+      </c>
+      <c r="H127" s="0">
+        <v>20.199999999999999</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0">
+        <v>0.00041378708156663299</v>
+      </c>
+      <c r="B128" s="0">
+        <v>0.00042448463195362987</v>
+      </c>
+      <c r="C128" s="0">
+        <v>0.00028473478194058718</v>
+      </c>
+      <c r="D128" s="0">
+        <v>0.00024319064967143702</v>
+      </c>
+      <c r="E128" s="0">
+        <v>0.00016929372878680523</v>
+      </c>
+      <c r="F128" s="0">
+        <v>0.00012460069601209908</v>
+      </c>
+      <c r="G128" s="0">
+        <v>1.824228755658202e-05</v>
+      </c>
+      <c r="H128" s="0">
+        <v>20.300000000000001</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0">
+        <v>0.00038376282909770846</v>
+      </c>
+      <c r="B129" s="0">
+        <v>0.00036097595321465877</v>
+      </c>
+      <c r="C129" s="0">
+        <v>0.00031096640651309617</v>
+      </c>
+      <c r="D129" s="0">
+        <v>0.00026928131260034178</v>
+      </c>
+      <c r="E129" s="0">
+        <v>0.00016104794860451703</v>
+      </c>
+      <c r="F129" s="0">
+        <v>0.00013288495477084623</v>
+      </c>
+      <c r="G129" s="0">
+        <v>1.9347511244878296e-05</v>
+      </c>
+      <c r="H129" s="0">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0">
+        <v>0.00042187544335182264</v>
+      </c>
+      <c r="B130" s="0">
+        <v>0.00039093559282772172</v>
+      </c>
+      <c r="C130" s="0">
+        <v>0.00028252524279334733</v>
+      </c>
+      <c r="D130" s="0">
+        <v>0.00024999799529348176</v>
+      </c>
+      <c r="E130" s="0">
+        <v>0.0001621066211818428</v>
+      </c>
+      <c r="F130" s="0">
+        <v>0.00013308714892742643</v>
+      </c>
+      <c r="G130" s="0">
+        <v>1.5003134306951252e-05</v>
+      </c>
+      <c r="H130" s="0">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0">
+        <v>0.0003871828654738752</v>
+      </c>
+      <c r="B131" s="0">
+        <v>0.00037154372527705153</v>
+      </c>
+      <c r="C131" s="0">
+        <v>0.0003396030549550627</v>
+      </c>
+      <c r="D131" s="0">
+        <v>0.00025781872525527998</v>
+      </c>
+      <c r="E131" s="0">
+        <v>0.0001688210294553972</v>
+      </c>
+      <c r="F131" s="0">
+        <v>0.00013846482500039895</v>
+      </c>
+      <c r="G131" s="0">
+        <v>1.2002590161856953e-05</v>
+      </c>
+      <c r="H131" s="0">
+        <v>20.600000000000001</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0">
+        <v>0.00043085233765042716</v>
+      </c>
+      <c r="B132" s="0">
+        <v>0.00037819065336362794</v>
+      </c>
+      <c r="C132" s="0">
+        <v>0.00028332445968963456</v>
+      </c>
+      <c r="D132" s="0">
+        <v>0.00026436500717624698</v>
+      </c>
+      <c r="E132" s="0">
+        <v>0.00015797161384160775</v>
+      </c>
+      <c r="F132" s="0">
+        <v>0.00015034149727199568</v>
+      </c>
+      <c r="G132" s="0">
+        <v>8.5612956049812498e-06</v>
+      </c>
+      <c r="H132" s="0">
+        <v>20.699999999999999</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0">
+        <v>0.00039149361122131447</v>
+      </c>
+      <c r="B133" s="0">
+        <v>0.00038359245943870484</v>
+      </c>
+      <c r="C133" s="0">
+        <v>0.00034011643811539868</v>
+      </c>
+      <c r="D133" s="0">
+        <v>0.00024986016418736306</v>
+      </c>
+      <c r="E133" s="0">
+        <v>0.0001795921596561774</v>
+      </c>
+      <c r="F133" s="0">
+        <v>0.00012304716506929478</v>
+      </c>
+      <c r="G133" s="0">
+        <v>5.9479945467813023e-06</v>
+      </c>
+      <c r="H133" s="0">
+        <v>20.800000000000001</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0">
+        <v>0.000440656893928742</v>
+      </c>
+      <c r="B134" s="0">
+        <v>0.00036735654284972887</v>
+      </c>
+      <c r="C134" s="0">
+        <v>0.0002863404383383508</v>
+      </c>
+      <c r="D134" s="0">
+        <v>0.00029174097821595135</v>
+      </c>
+      <c r="E134" s="0">
+        <v>0.00015675414454324827</v>
+      </c>
+      <c r="F134" s="0">
+        <v>0.00014150962254996257</v>
+      </c>
+      <c r="G134" s="0">
+        <v>3.65434697980964e-06</v>
+      </c>
+      <c r="H134" s="0">
+        <v>20.899999999999999</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0">
+        <v>0.00039747572029880909</v>
+      </c>
+      <c r="B135" s="0">
+        <v>0.00039803527544867643</v>
+      </c>
+      <c r="C135" s="0">
+        <v>0.00031178624641719452</v>
+      </c>
+      <c r="D135" s="0">
+        <v>0.00024435826845741994</v>
+      </c>
+      <c r="E135" s="0">
+        <v>0.00019891575942469444</v>
+      </c>
+      <c r="F135" s="0">
+        <v>0.00011915207541288422</v>
+      </c>
+      <c r="G135" s="0">
+        <v>1.2581511427118601e-06</v>
+      </c>
+      <c r="H135" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0">
+        <v>0.0003797444405846567</v>
+      </c>
+      <c r="B136" s="0">
+        <v>0.00034357206672406372</v>
+      </c>
+      <c r="C136" s="0">
+        <v>0.00028577342983141126</v>
+      </c>
+      <c r="D136" s="0">
+        <v>0.00030739</v>
+      </c>
+      <c r="E136" s="0">
+        <v>0.00015743501598607446</v>
+      </c>
+      <c r="F136" s="0">
+        <v>0.00011956667471726626</v>
+      </c>
+      <c r="G136" s="0">
+        <v>6.9159639995952087e-07</v>
+      </c>
+      <c r="H136" s="0">
+        <v>21.100000000000001</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0">
+        <v>0.00040361689607648296</v>
+      </c>
+      <c r="B137" s="0">
+        <v>0.00042464576502440464</v>
+      </c>
+      <c r="C137" s="0">
+        <v>0.0002956663613593573</v>
+      </c>
+      <c r="D137" s="0">
+        <v>0.00024159210081356699</v>
+      </c>
+      <c r="E137" s="0">
+        <v>0.00018544957728718945</v>
+      </c>
+      <c r="F137" s="0">
+        <v>0.00012018742877616202</v>
+      </c>
+      <c r="G137" s="0">
+        <v>9.725499999999999e-07</v>
+      </c>
+      <c r="H137" s="0">
+        <v>21.199999999999999</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="0">
+        <v>0.0003809660629158037</v>
+      </c>
+      <c r="B138" s="0">
+        <v>0.00035087026423925172</v>
+      </c>
+      <c r="C138" s="0">
+        <v>0.00029326027649308325</v>
+      </c>
+      <c r="D138" s="0">
+        <v>0.00028618686855615854</v>
+      </c>
+      <c r="E138" s="0">
+        <v>0.00015722776997318088</v>
+      </c>
+      <c r="F138" s="0">
+        <v>0.00012195751661074543</v>
+      </c>
+      <c r="G138" s="0">
+        <v>4.7116345977890171e-06</v>
+      </c>
+      <c r="H138" s="0">
+        <v>21.300000000000001</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="0">
+        <v>0.00041035747155033239</v>
+      </c>
+      <c r="B139" s="0">
+        <v>0.00042448388123875755</v>
+      </c>
+      <c r="C139" s="0">
+        <v>0.00028707223020498163</v>
+      </c>
+      <c r="D139" s="0">
+        <v>0.00024171529659168208</v>
+      </c>
+      <c r="E139" s="0">
+        <v>0.00017383658756468307</v>
+      </c>
+      <c r="F139" s="0">
+        <v>0.00012448773544132324</v>
+      </c>
+      <c r="G139" s="0">
+        <v>8.430192142771746e-06</v>
+      </c>
+      <c r="H139" s="0">
+        <v>21.399999999999999</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="0">
+        <v>0.00038319494903305099</v>
+      </c>
+      <c r="B140" s="0">
+        <v>0.0003593751449620789</v>
+      </c>
+      <c r="C140" s="0">
+        <v>0.00030753489284978986</v>
+      </c>
+      <c r="D140" s="0">
+        <v>0.00027074786559491768</v>
+      </c>
+      <c r="E140" s="0">
+        <v>0.00016051914483186972</v>
+      </c>
+      <c r="F140" s="0">
+        <v>0.00013222268156095837</v>
+      </c>
+      <c r="G140" s="0">
+        <v>1.2600715313424414e-05</v>
+      </c>
+      <c r="H140" s="0">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="0">
+        <v>0.00041764326938574698</v>
+      </c>
+      <c r="B141" s="0">
+        <v>0.00039820064724569696</v>
+      </c>
+      <c r="C141" s="0">
+        <v>0.00028313476522883293</v>
+      </c>
+      <c r="D141" s="0">
+        <v>0.00024583944851884232</v>
+      </c>
+      <c r="E141" s="0">
+        <v>0.00016558538425519794</v>
+      </c>
+      <c r="F141" s="0">
+        <v>0.00013085054366301249</v>
+      </c>
+      <c r="G141" s="0">
+        <v>1.5168913096303569e-05</v>
+      </c>
+      <c r="H141" s="0">
+        <v>21.600000000000001</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="0">
+        <v>0.00038635419994989138</v>
+      </c>
+      <c r="B142" s="0">
+        <v>0.0003690735522066414</v>
+      </c>
+      <c r="C142" s="0">
+        <v>0.00033218613670190874</v>
+      </c>
+      <c r="D142" s="0">
+        <v>0.0002600973316340633</v>
+      </c>
+      <c r="E142" s="0">
+        <v>0.0001676841002176234</v>
+      </c>
+      <c r="F142" s="0">
+        <v>0.00014422095733116416</v>
+      </c>
+      <c r="G142" s="0">
+        <v>1.9473161581188467e-05</v>
+      </c>
+      <c r="H142" s="0">
+        <v>21.699999999999999</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="0">
+        <v>0.00042570267560940335</v>
+      </c>
+      <c r="B143" s="0">
+        <v>0.00038497430027418052</v>
+      </c>
+      <c r="C143" s="0">
+        <v>0.00028249763809656424</v>
+      </c>
+      <c r="D143" s="0">
+        <v>0.00025600024462552582</v>
+      </c>
+      <c r="E143" s="0">
+        <v>0.00016021270751400584</v>
+      </c>
+      <c r="F143" s="0">
+        <v>0.00013980811335005265</v>
+      </c>
+      <c r="G143" s="0">
+        <v>2.1558839395057611e-05</v>
+      </c>
+      <c r="H143" s="0">
+        <v>21.800000000000001</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="0">
+        <v>0.00039023478888633022</v>
+      </c>
+      <c r="B144" s="0">
+        <v>0.00038020383533981958</v>
+      </c>
+      <c r="C144" s="0">
+        <v>0.00035023304669740395</v>
+      </c>
+      <c r="D144" s="0">
+        <v>0.0002516478799932222</v>
+      </c>
+      <c r="E144" s="0">
+        <v>0.00017680605361869182</v>
+      </c>
+      <c r="F144" s="0">
+        <v>0.00012721930476823086</v>
+      </c>
+      <c r="G144" s="0">
+        <v>2.4767148855892695e-05</v>
+      </c>
+      <c r="H144" s="0">
+        <v>21.899999999999999</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="0">
         <v>0.00043438851066310768</v>
       </c>
-      <c r="B122" s="0">
+      <c r="B145" s="0">
         <v>0.00037374948608279586</v>
       </c>
-      <c r="C122" s="0">
+      <c r="C145" s="0">
         <v>0.00028423305165511438</v>
       </c>
-      <c r="D122" s="0">
+      <c r="D145" s="0">
         <v>0.00027266245976642612</v>
       </c>
-      <c r="E122" s="0">
+      <c r="E145" s="0">
         <v>0.00015750679474757048</v>
       </c>
-      <c r="F122" s="0">
+      <c r="F145" s="0">
         <v>0.00015188025604551437</v>
       </c>
-      <c r="G122" s="0">
+      <c r="G145" s="0">
         <v>2.8574713720893019e-05</v>
       </c>
-      <c r="H122" s="0">
+      <c r="H145" s="0">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rest of the FEA analysis for the beam
</commit_message>
<xml_diff>
--- a/data/runsMarch/InterpolatedResults.xlsx
+++ b/data/runsMarch/InterpolatedResults.xlsx
@@ -82,7 +82,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:H240"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2804,1068 +2804,3538 @@
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>0.00038182392884372258</v>
+        <v>0.00042811074952831056</v>
       </c>
       <c r="B105" s="0">
-        <v>0.00035403039842678725</v>
+        <v>0.00034306804672484586</v>
       </c>
       <c r="C105" s="0">
-        <v>0.00029786839697544439</v>
+        <v>0.00022746202156250243</v>
       </c>
       <c r="D105" s="0">
-        <v>0.00028047487531956641</v>
+        <v>8.8715305566088308e-05</v>
       </c>
       <c r="E105" s="0">
-        <v>0.00015149541401110123</v>
+        <v>0.0001571789784146284</v>
       </c>
       <c r="F105" s="0">
-        <v>7.3537178411631562e-05</v>
+        <v>0.00015348959572248131</v>
       </c>
       <c r="G105" s="0">
-        <v>4.7948218254677212e-05</v>
+        <v>4.7663175942709221e-05</v>
       </c>
       <c r="H105" s="0">
-        <v>18</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>0.00042263658554286913</v>
+        <v>0.0003974367184576569</v>
       </c>
       <c r="B106" s="0">
-        <v>0.00039022460742583592</v>
+        <v>0.00039148955024707508</v>
       </c>
       <c r="C106" s="0">
-        <v>0.0002824991476365973</v>
+        <v>0.00022885661796171863</v>
       </c>
       <c r="D106" s="0">
-        <v>0.00025123454853737641</v>
+        <v>7.6745072108125146e-05</v>
       </c>
       <c r="E106" s="0">
-        <v>0.00015649654231147101</v>
+        <v>0.00015702729943528393</v>
       </c>
       <c r="F106" s="0">
-        <v>8.6109326009228211e-05</v>
+        <v>0.00012179737148585232</v>
       </c>
       <c r="G106" s="0">
-        <v>4.4668336411425145e-05</v>
+        <v>4.9970711963348897e-05</v>
       </c>
       <c r="H106" s="0">
-        <v>18.100000000000001</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0">
-        <v>0.00038507274854935063</v>
+        <v>0.00039844392879587252</v>
       </c>
       <c r="B107" s="0">
-        <v>0.00036483926768487594</v>
+        <v>0.00032822684064196493</v>
       </c>
       <c r="C107" s="0">
-        <v>0.00031992875715390091</v>
+        <v>0.00022845202935630883</v>
       </c>
       <c r="D107" s="0">
-        <v>0.00026506155257288694</v>
+        <v>5.6787278116039581e-05</v>
       </c>
       <c r="E107" s="0">
-        <v>0.0001591575848330936</v>
+        <v>0.00016039827430592128</v>
       </c>
       <c r="F107" s="0">
-        <v>9.78150678888276e-05</v>
+        <v>0.00014402102564001256</v>
       </c>
       <c r="G107" s="0">
-        <v>4.9136529576521611e-05</v>
+        <v>4.7788936488460581e-05</v>
       </c>
       <c r="H107" s="0">
-        <v>18.199999999999999</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>0.0004327808641336705</v>
+        <v>0.00041045027279351339</v>
       </c>
       <c r="B108" s="0">
-        <v>0.0003758961980946703</v>
+        <v>0.00041934511425238046</v>
       </c>
       <c r="C108" s="0">
-        <v>0.00028380656905634393</v>
+        <v>0.00022604445352582324</v>
       </c>
       <c r="D108" s="0">
-        <v>0.00026968978035771517</v>
+        <v>3.8411768394855172e-05</v>
       </c>
       <c r="E108" s="0">
-        <v>0.00015331144650088585</v>
+        <v>0.00017995221444922789</v>
       </c>
       <c r="F108" s="0">
-        <v>0.0001087361715420914</v>
+        <v>0.00012537100873147766</v>
       </c>
       <c r="G108" s="0">
-        <v>4.3458412126515643e-05</v>
+        <v>4.8149859886691856e-05</v>
       </c>
       <c r="H108" s="0">
-        <v>18.300000000000001</v>
+        <v>10.699999999999999</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>0.00038938738530532144</v>
+        <v>0.00038454189722536986</v>
       </c>
       <c r="B109" s="0">
-        <v>0.00037742531329545569</v>
+        <v>0.00032757076851580531</v>
       </c>
       <c r="C109" s="0">
-        <v>0.00036146000000000003</v>
+        <v>0.00023336361246297684</v>
       </c>
       <c r="D109" s="0">
-        <v>0.00025353881884849821</v>
+        <v>2.5328085742872175e-05</v>
       </c>
       <c r="E109" s="0">
-        <v>0.000169765067159418</v>
+        <v>0.0001714927406625656</v>
       </c>
       <c r="F109" s="0">
-        <v>9.6568531907344939e-05</v>
+        <v>0.00013712489374810796</v>
       </c>
       <c r="G109" s="0">
-        <v>5.1150164233478986e-05</v>
+        <v>4.8058683683155296e-05</v>
       </c>
       <c r="H109" s="0">
-        <v>18.399999999999999</v>
+        <v>10.800000000000001</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0">
-        <v>0.00044421328440124344</v>
+        <v>0.0004259127623507971</v>
       </c>
       <c r="B110" s="0">
-        <v>0.0003642544185057215</v>
+        <v>0.00038137480397017616</v>
       </c>
       <c r="C110" s="0">
-        <v>0.00028782486224797951</v>
+        <v>0.00023467071034032039</v>
       </c>
       <c r="D110" s="0">
-        <v>0.00030739999999999999</v>
+        <v>9.2175322481846434e-06</v>
       </c>
       <c r="E110" s="0">
-        <v>0.0001540231045654136</v>
+        <v>0.00017020986983633314</v>
       </c>
       <c r="F110" s="0">
-        <v>0.00010757903629168223</v>
+        <v>0.00012907556830320173</v>
       </c>
       <c r="G110" s="0">
-        <v>4.2544425759221937e-05</v>
+        <v>4.7756565753868742e-05</v>
       </c>
       <c r="H110" s="0">
-        <v>18.5</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>0.000395478019881029</v>
+        <v>0.00037992274079385409</v>
       </c>
       <c r="B111" s="0">
-        <v>0.00039237312034107684</v>
+        <v>0.0003345840900135665</v>
       </c>
       <c r="C111" s="0">
-        <v>0.00032062359078040476</v>
+        <v>0.00024140104069293825</v>
       </c>
       <c r="D111" s="0">
-        <v>0.00024596695212480594</v>
+        <v>3.9925832990796992e-06</v>
       </c>
       <c r="E111" s="0">
-        <v>0.00018491724810573763</v>
+        <v>0.00019877</v>
       </c>
       <c r="F111" s="0">
-        <v>9.6163265471782165e-05</v>
+        <v>0.00013101169428202523</v>
       </c>
       <c r="G111" s="0">
-        <v>5.2483345942018852e-05</v>
+        <v>4.8328286174147858e-05</v>
       </c>
       <c r="H111" s="0">
-        <v>18.600000000000001</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>0.00037988763299700456</v>
+        <v>0.00044432123117443991</v>
       </c>
       <c r="B112" s="0">
-        <v>0.00033764902196670046</v>
+        <v>0.00036149234537655276</v>
       </c>
       <c r="C112" s="0">
-        <v>0.0002831291216530299</v>
+        <v>0.00024971862079727628</v>
       </c>
       <c r="D112" s="0">
-        <v>0.00028825940875697485</v>
+        <v>4.5425000000000001e-06</v>
       </c>
       <c r="E112" s="0">
-        <v>0.00016141810289328301</v>
+        <v>0.00016255596515690846</v>
       </c>
       <c r="F112" s="0">
-        <v>0.00010083520724207844</v>
+        <v>0.00013432405626277226</v>
       </c>
       <c r="G112" s="0">
-        <v>4.1923998804146153e-05</v>
+        <v>4.7637642916636627e-05</v>
       </c>
       <c r="H112" s="0">
-        <v>18.699999999999999</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0">
-        <v>0.00040208612668883972</v>
+        <v>0.00038099012138254133</v>
       </c>
       <c r="B113" s="0">
-        <v>0.00042482068432186606</v>
+        <v>0.00034791451180362894</v>
       </c>
       <c r="C113" s="0">
-        <v>0.00029889649533664599</v>
+        <v>0.00025891362670905064</v>
       </c>
       <c r="D113" s="0">
-        <v>0.00024201213489089728</v>
+        <v>2.1467574837472351e-05</v>
       </c>
       <c r="E113" s="0">
-        <v>0.00018675160468337106</v>
+        <v>0.00016894091096437909</v>
       </c>
       <c r="F113" s="0">
-        <v>0.00010102874000619502</v>
+        <v>0.00012616976776340193</v>
       </c>
       <c r="G113" s="0">
-        <v>4.6006869579689803e-05</v>
+        <v>4.8777270411311572e-05</v>
       </c>
       <c r="H113" s="0">
-        <v>18.800000000000001</v>
+        <v>11.199999999999999</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>0.00037988915471760571</v>
+        <v>0.00046263011516132981</v>
       </c>
       <c r="B114" s="0">
-        <v>0.00034450036034599114</v>
+        <v>0.00037318152724340534</v>
       </c>
       <c r="C114" s="0">
-        <v>0.00028649627340217283</v>
+        <v>0.00032607313298742741</v>
       </c>
       <c r="D114" s="0">
-        <v>0.00030737098996192326</v>
+        <v>3.8619837283071378e-05</v>
       </c>
       <c r="E114" s="0">
-        <v>0.00015511119957767403</v>
+        <v>0.00015728243698357301</v>
       </c>
       <c r="F114" s="0">
-        <v>0.00010359665977772487</v>
+        <v>0.00014042643017180445</v>
       </c>
       <c r="G114" s="0">
-        <v>4.161672214846615e-05</v>
+        <v>4.7567060967684562e-05</v>
       </c>
       <c r="H114" s="0">
-        <v>18.899999999999999</v>
+        <v>11.300000000000001</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>0.00040953265912630729</v>
+        <v>0.00038596221605461886</v>
       </c>
       <c r="B115" s="0">
-        <v>0.00042463236636216303</v>
+        <v>0.000365305292640496</v>
       </c>
       <c r="C115" s="0">
-        <v>0.00028788027265744584</v>
+        <v>0.00029791708778700155</v>
       </c>
       <c r="D115" s="0">
-        <v>0.00024149277651625922</v>
+        <v>5.8893212653264335e-05</v>
       </c>
       <c r="E115" s="0">
-        <v>0.0001736803913727378</v>
+        <v>0.00015725746675500241</v>
       </c>
       <c r="F115" s="0">
-        <v>0.00010850719496213222</v>
+        <v>0.00012327415332609307</v>
       </c>
       <c r="G115" s="0">
-        <v>4.1706947000387257e-05</v>
+        <v>4.9479419007308293e-05</v>
       </c>
       <c r="H115" s="0">
-        <v>19</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0">
-        <v>0.00038151463633301439</v>
+        <v>0.00041822737551753652</v>
       </c>
       <c r="B116" s="0">
-        <v>0.00035289061045873989</v>
+        <v>0.00034204725016972223</v>
       </c>
       <c r="C116" s="0">
-        <v>0.00029604826280225845</v>
+        <v>0.00029272940801276136</v>
       </c>
       <c r="D116" s="0">
-        <v>0.00028235815716253578</v>
+        <v>7.1392361992495668e-05</v>
       </c>
       <c r="E116" s="0">
-        <v>0.00015589537214092853</v>
+        <v>0.00015452753380587939</v>
       </c>
       <c r="F116" s="0">
-        <v>0.00011065198203045973</v>
+        <v>0.00015353601210985393</v>
       </c>
       <c r="G116" s="0">
-        <v>4.132260987058966e-05</v>
+        <v>4.7614565840428503e-05</v>
       </c>
       <c r="H116" s="0">
-        <v>19.100000000000001</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>0.0004177687477483571</v>
+        <v>0.00039436866994056177</v>
       </c>
       <c r="B117" s="0">
-        <v>0.00039832923599365545</v>
+        <v>0.00038783146759082543</v>
       </c>
       <c r="C117" s="0">
-        <v>0.00028320127519340432</v>
+        <v>0.00030514660803896722</v>
       </c>
       <c r="D117" s="0">
-        <v>0.0002458344506389971</v>
+        <v>9.1577981800929667e-05</v>
       </c>
       <c r="E117" s="0">
-        <v>0.00016401626080857697</v>
+        <v>0.0001540699619400233</v>
       </c>
       <c r="F117" s="0">
-        <v>0.00011891532946045304</v>
+        <v>0.00012144990944166619</v>
       </c>
       <c r="G117" s="0">
-        <v>3.7914432128473924e-05</v>
+        <v>5.0140143144628886e-05</v>
       </c>
       <c r="H117" s="0">
-        <v>19.199999999999999</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>0.0003843650390263374</v>
+        <v>0.00039500193374729831</v>
       </c>
       <c r="B118" s="0">
-        <v>0.00036279192915659179</v>
+        <v>0.00033116643615076251</v>
       </c>
       <c r="C118" s="0">
-        <v>0.00031505567726572263</v>
+        <v>0.00027936308069127704</v>
       </c>
       <c r="D118" s="0">
-        <v>0.00026760875237498725</v>
+        <v>0.00010348472583253183</v>
       </c>
       <c r="E118" s="0">
-        <v>0.00016127307586172047</v>
+        <v>0.00015596302860333721</v>
       </c>
       <c r="F118" s="0">
-        <v>0.00012749704438623597</v>
+        <v>0.00014601233154248045</v>
       </c>
       <c r="G118" s="0">
-        <v>4.122909806432214e-05</v>
+        <v>4.7785244929208619e-05</v>
       </c>
       <c r="H118" s="0">
-        <v>19.300000000000001</v>
+        <v>11.699999999999999</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0">
-        <v>0.00042698230145499152</v>
+        <v>0.00040517677153964829</v>
       </c>
       <c r="B119" s="0">
-        <v>0.00038360380828790546</v>
+        <v>0.00042374842495612741</v>
       </c>
       <c r="C119" s="0">
-        <v>0.00028267210479419847</v>
+        <v>0.00027787552027951231</v>
       </c>
       <c r="D119" s="0">
-        <v>0.00025786451662419764</v>
+        <v>0.00011694676342547652</v>
       </c>
       <c r="E119" s="0">
-        <v>0.00015857461803323489</v>
+        <v>0.00015529848302121285</v>
       </c>
       <c r="F119" s="0">
-        <v>0.00013106221553029531</v>
+        <v>0.00012191721850318838</v>
       </c>
       <c r="G119" s="0">
-        <v>3.4659511520834067e-05</v>
+        <v>5.0887974437428753e-05</v>
       </c>
       <c r="H119" s="0">
-        <v>19.399999999999999</v>
+        <v>11.800000000000001</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>0.00038824260111763263</v>
+        <v>0.00038389216475763027</v>
       </c>
       <c r="B120" s="0">
-        <v>0.00037412402798497554</v>
+        <v>0.00033098846610763588</v>
       </c>
       <c r="C120" s="0">
-        <v>0.00034913908421271633</v>
+        <v>0.00027309709194389974</v>
       </c>
       <c r="D120" s="0">
-        <v>0.00025563690795786422</v>
+        <v>0.00013975711280533491</v>
       </c>
       <c r="E120" s="0">
-        <v>0.00017032375255516448</v>
+        <v>0.00016544695970078472</v>
       </c>
       <c r="F120" s="0">
-        <v>0.0001269646056787803</v>
+        <v>0.00013758522324183105</v>
       </c>
       <c r="G120" s="0">
-        <v>4.1314984616979181e-05</v>
+        <v>4.7961538036952546e-05</v>
       </c>
       <c r="H120" s="0">
-        <v>19.5</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>0.00043689789063666772</v>
+        <v>0.00041799517197154491</v>
       </c>
       <c r="B121" s="0">
-        <v>0.00037119469745727378</v>
+        <v>0.00039762678208308296</v>
       </c>
       <c r="C121" s="0">
-        <v>0.00028499719891668499</v>
+        <v>0.00027144222889523761</v>
       </c>
       <c r="D121" s="0">
-        <v>0.00027943614250291402</v>
+        <v>0.00014292878311933304</v>
       </c>
       <c r="E121" s="0">
-        <v>0.00015604071960330259</v>
+        <v>0.00017094272156173377</v>
       </c>
       <c r="F121" s="0">
-        <v>0.00014391932939816443</v>
+        <v>0.00012632288302721212</v>
       </c>
       <c r="G121" s="0">
-        <v>3.1747541055753856e-05</v>
+        <v>4.7898638888926668e-05</v>
       </c>
       <c r="H121" s="0">
-        <v>19.600000000000001</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0">
-        <v>0.00039302186621724362</v>
+        <v>0.00038006175105245174</v>
       </c>
       <c r="B122" s="0">
-        <v>0.00038760809623591323</v>
+        <v>0.00033701777515382075</v>
       </c>
       <c r="C122" s="0">
-        <v>0.00032998932637252844</v>
+        <v>0.00027298441470301432</v>
       </c>
       <c r="D122" s="0">
-        <v>0.0002479592542960384</v>
+        <v>0.00018051039413307523</v>
       </c>
       <c r="E122" s="0">
-        <v>0.00018223999991138663</v>
+        <v>0.00019196</v>
       </c>
       <c r="F122" s="0">
-        <v>0.00011671766886766412</v>
+        <v>0.00013065719522087888</v>
       </c>
       <c r="G122" s="0">
-        <v>3.3955822806207834e-05</v>
+        <v>4.8310460590123296e-05</v>
       </c>
       <c r="H122" s="0">
-        <v>19.699999999999999</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0">
-        <v>0.00037983548707013382</v>
+        <v>0.00043299227949115005</v>
       </c>
       <c r="B123" s="0">
-        <v>0.00033760889927089862</v>
+        <v>0.00037535654930302378</v>
       </c>
       <c r="C123" s="0">
-        <v>0.00028311314861404206</v>
+        <v>0.00027468893090777191</v>
       </c>
       <c r="D123" s="0">
-        <v>0.0002882853969048376</v>
+        <v>0.00017922578690732612</v>
       </c>
       <c r="E123" s="0">
-        <v>0.00016347221474073315</v>
+        <v>0.00015929281848710229</v>
       </c>
       <c r="F123" s="0">
-        <v>0.00011742811815592588</v>
+        <v>0.00013085888877066543</v>
       </c>
       <c r="G123" s="0">
-        <v>2.8937451254732675e-05</v>
+        <v>4.7700964199067269e-05</v>
       </c>
       <c r="H123" s="0">
-        <v>19.800000000000001</v>
+        <v>12.199999999999999</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0">
-        <v>0.00039958924597638374</v>
+        <v>0.00038079938112726237</v>
       </c>
       <c r="B124" s="0">
-        <v>0.00040377288248296436</v>
+        <v>0.00034840224990181727</v>
       </c>
       <c r="C124" s="0">
-        <v>0.00030492034402949817</v>
+        <v>0.00028276489402994406</v>
       </c>
       <c r="D124" s="0">
-        <v>0.00024303134599600778</v>
+        <v>0.00020261026468572217</v>
       </c>
       <c r="E124" s="0">
-        <v>0.00019827081250733467</v>
+        <v>0.00016010325072200163</v>
       </c>
       <c r="F124" s="0">
-        <v>0.00011545632363013652</v>
+        <v>0.00012532512695971989</v>
       </c>
       <c r="G124" s="0">
-        <v>2.7963381969978955e-05</v>
+        <v>4.8753914720547597e-05</v>
       </c>
       <c r="H124" s="0">
-        <v>19.899999999999999</v>
+        <v>12.300000000000001</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0">
-        <v>0.00037983098980074289</v>
+        <v>0.00044435469115576678</v>
       </c>
       <c r="B125" s="0">
-        <v>0.00034398992418763235</v>
+        <v>0.00036087640941452213</v>
       </c>
       <c r="C125" s="0">
-        <v>0.00028608230498257907</v>
+        <v>0.00032860789920624854</v>
       </c>
       <c r="D125" s="0">
-        <v>0.0003074004775742926</v>
+        <v>0.0001786966771115917</v>
       </c>
       <c r="E125" s="0">
-        <v>0.00015706290094026192</v>
+        <v>0.00015074475500487133</v>
       </c>
       <c r="F125" s="0">
-        <v>0.0001163716197775485</v>
+        <v>0.00013741254377609919</v>
       </c>
       <c r="G125" s="0">
-        <v>2.5848217007533918e-05</v>
+        <v>4.7561872919635698e-05</v>
       </c>
       <c r="H125" s="0">
-        <v>20</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0">
-        <v>0.0004063478779601894</v>
+        <v>0.00038482710543282493</v>
       </c>
       <c r="B126" s="0">
-        <v>0.00042464983324247402</v>
+        <v>0.0003634002605734085</v>
       </c>
       <c r="C126" s="0">
-        <v>0.00029142654136816136</v>
+        <v>0.00031093632090876207</v>
       </c>
       <c r="D126" s="0">
-        <v>0.00024125164485324738</v>
+        <v>0.0002024204732268804</v>
       </c>
       <c r="E126" s="0">
-        <v>0.00018026720262323309</v>
+        <v>0.00014755438387614668</v>
       </c>
       <c r="F126" s="0">
-        <v>0.00011845174607069648</v>
+        <v>0.0001220842182447385</v>
       </c>
       <c r="G126" s="0">
-        <v>2.275058031244153e-05</v>
+        <v>4.9632670912153506e-05</v>
       </c>
       <c r="H126" s="0">
-        <v>20.100000000000001</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0">
-        <v>0.00038120676550941756</v>
+        <v>0.00041111522793752306</v>
       </c>
       <c r="B127" s="0">
-        <v>0.00035179326377914581</v>
+        <v>0.00033904613566507094</v>
       </c>
       <c r="C127" s="0">
-        <v>0.00029452938714597578</v>
+        <v>0.00030587064738863464</v>
       </c>
       <c r="D127" s="0">
-        <v>0.00028425145520624473</v>
+        <v>0.00018931575607687807</v>
       </c>
       <c r="E127" s="0">
-        <v>0.00015697971490512307</v>
+        <v>0.00014475669106955082</v>
       </c>
       <c r="F127" s="0">
-        <v>0.00011984659736553046</v>
+        <v>0.00014556804631301695</v>
       </c>
       <c r="G127" s="0">
-        <v>2.2644821219429934e-05</v>
+        <v>4.7568206759935083e-05</v>
       </c>
       <c r="H127" s="0">
-        <v>20.199999999999999</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0">
-        <v>0.00041378708156663299</v>
+        <v>0.0003914107119261861</v>
       </c>
       <c r="B128" s="0">
-        <v>0.00042448463195362987</v>
+        <v>0.00038229064233140961</v>
       </c>
       <c r="C128" s="0">
-        <v>0.00028473478194058718</v>
+        <v>0.00033820040611825169</v>
       </c>
       <c r="D128" s="0">
-        <v>0.00024319064967143702</v>
+        <v>0.00020217237063098161</v>
       </c>
       <c r="E128" s="0">
-        <v>0.00016929372878680523</v>
+        <v>0.00014321373136344425</v>
       </c>
       <c r="F128" s="0">
-        <v>0.00012460069601209908</v>
+        <v>0.00012030867166653545</v>
       </c>
       <c r="G128" s="0">
-        <v>1.824228755658202e-05</v>
+        <v>5.0310606685121409e-05</v>
       </c>
       <c r="H128" s="0">
-        <v>20.300000000000001</v>
+        <v>12.699999999999999</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0">
-        <v>0.00038376282909770846</v>
+        <v>0.00039264053334057243</v>
       </c>
       <c r="B129" s="0">
-        <v>0.00036097595321465877</v>
+        <v>0.00033145780168405324</v>
       </c>
       <c r="C129" s="0">
-        <v>0.00031096640651309617</v>
+        <v>0.00029059655287532084</v>
       </c>
       <c r="D129" s="0">
-        <v>0.00026928131260034178</v>
+        <v>0.00020664559212646929</v>
       </c>
       <c r="E129" s="0">
-        <v>0.00016104794860451703</v>
+        <v>0.00014209669071358331</v>
       </c>
       <c r="F129" s="0">
-        <v>0.00013288495477084623</v>
+        <v>0.00015232682234697574</v>
       </c>
       <c r="G129" s="0">
-        <v>1.9347511244878296e-05</v>
+        <v>4.769977718707646e-05</v>
       </c>
       <c r="H129" s="0">
-        <v>20.399999999999999</v>
+        <v>12.800000000000001</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0">
-        <v>0.00042187544335182264</v>
+        <v>0.00040110551125587131</v>
       </c>
       <c r="B130" s="0">
-        <v>0.00039093559282772172</v>
+        <v>0.0004247746588316714</v>
       </c>
       <c r="C130" s="0">
-        <v>0.00028252524279334733</v>
+        <v>0.00029812802309271707</v>
       </c>
       <c r="D130" s="0">
-        <v>0.00024999799529348176</v>
+        <v>0.00020696212818329957</v>
       </c>
       <c r="E130" s="0">
-        <v>0.0001621066211818428</v>
+        <v>0.00014294828889297603</v>
       </c>
       <c r="F130" s="0">
-        <v>0.00013308714892742643</v>
+        <v>0.00012189526022226596</v>
       </c>
       <c r="G130" s="0">
-        <v>1.5003134306951252e-05</v>
+        <v>5.1304704269209711e-05</v>
       </c>
       <c r="H130" s="0">
-        <v>20.5</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0">
-        <v>0.0003871828654738752</v>
+        <v>0.00038336427273767844</v>
       </c>
       <c r="B131" s="0">
-        <v>0.00037154372527705153</v>
+        <v>0.0003319727613119977</v>
       </c>
       <c r="C131" s="0">
-        <v>0.0003396030549550627</v>
+        <v>0.00028258309935686392</v>
       </c>
       <c r="D131" s="0">
-        <v>0.00025781872525527998</v>
+        <v>0.00022978167803450566</v>
       </c>
       <c r="E131" s="0">
-        <v>0.0001688210294553972</v>
+        <v>0.00014581731977159718</v>
       </c>
       <c r="F131" s="0">
-        <v>0.00013846482500039895</v>
+        <v>0.00013706373380735319</v>
       </c>
       <c r="G131" s="0">
-        <v>1.2002590161856953e-05</v>
+        <v>4.7941393009115541e-05</v>
       </c>
       <c r="H131" s="0">
-        <v>20.600000000000001</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0">
-        <v>0.00043085233765042716</v>
+        <v>0.00041190343111270177</v>
       </c>
       <c r="B132" s="0">
-        <v>0.00037819065336362794</v>
+        <v>0.00042458765997208504</v>
       </c>
       <c r="C132" s="0">
-        <v>0.00028332445968963456</v>
+        <v>0.00028322557158033787</v>
       </c>
       <c r="D132" s="0">
-        <v>0.00026436500717624698</v>
+        <v>0.00021397492856689885</v>
       </c>
       <c r="E132" s="0">
-        <v>0.00015797161384160775</v>
+        <v>0.00014590485974042558</v>
       </c>
       <c r="F132" s="0">
-        <v>0.00015034149727199568</v>
+        <v>0.00012860337327901314</v>
       </c>
       <c r="G132" s="0">
-        <v>8.5612956049812498e-06</v>
+        <v>5.2193933310504639e-05</v>
       </c>
       <c r="H132" s="0">
-        <v>20.699999999999999</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0">
-        <v>0.00039149361122131447</v>
+        <v>0.00038006976225219899</v>
       </c>
       <c r="B133" s="0">
-        <v>0.00038359245943870484</v>
+        <v>0.00033757099204648845</v>
       </c>
       <c r="C133" s="0">
-        <v>0.00034011643811539868</v>
+        <v>0.00028070123020713705</v>
       </c>
       <c r="D133" s="0">
-        <v>0.00024986016418736306</v>
+        <v>0.00026011450326736629</v>
       </c>
       <c r="E133" s="0">
-        <v>0.0001795921596561774</v>
+        <v>0.00016627999999999999</v>
       </c>
       <c r="F133" s="0">
-        <v>0.00012304716506929478</v>
+        <v>0.00012895046814002535</v>
       </c>
       <c r="G133" s="0">
-        <v>5.9479945467813023e-06</v>
+        <v>4.8282805488485092e-05</v>
       </c>
       <c r="H133" s="0">
-        <v>20.800000000000001</v>
+        <v>13.199999999999999</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0">
-        <v>0.000440656893928742</v>
+        <v>0.00042465026208757901</v>
       </c>
       <c r="B134" s="0">
-        <v>0.00036735654284972887</v>
+        <v>0.00038736785482336959</v>
       </c>
       <c r="C134" s="0">
-        <v>0.0002863404383383508</v>
+        <v>0.00028034555146006288</v>
       </c>
       <c r="D134" s="0">
-        <v>0.00029174097821595135</v>
+        <v>0.00023027750345542986</v>
       </c>
       <c r="E134" s="0">
-        <v>0.00015675414454324827</v>
+        <v>0.0001399696490189843</v>
       </c>
       <c r="F134" s="0">
-        <v>0.00014150962254996257</v>
+        <v>0.00012615729703269798</v>
       </c>
       <c r="G134" s="0">
-        <v>3.65434697980964e-06</v>
+        <v>4.7804745760296919e-05</v>
       </c>
       <c r="H134" s="0">
-        <v>20.899999999999999</v>
+        <v>13.300000000000001</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0">
-        <v>0.00039747572029880909</v>
+        <v>0.00038058088593654655</v>
       </c>
       <c r="B135" s="0">
-        <v>0.00039803527544867643</v>
+        <v>0.00034773521710269298</v>
       </c>
       <c r="C135" s="0">
-        <v>0.00031178624641719452</v>
+        <v>0.00028766594978759844</v>
       </c>
       <c r="D135" s="0">
-        <v>0.00024435826845741994</v>
+        <v>0.00027215178375354437</v>
       </c>
       <c r="E135" s="0">
-        <v>0.00019891575942469444</v>
+        <v>0.00013248645115563015</v>
       </c>
       <c r="F135" s="0">
-        <v>0.00011915207541288422</v>
+        <v>0.00012273389796275784</v>
       </c>
       <c r="G135" s="0">
-        <v>1.2581511427118601e-06</v>
+        <v>4.8835051154204932e-05</v>
       </c>
       <c r="H135" s="0">
-        <v>21</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0">
-        <v>0.0003797444405846567</v>
+        <v>0.00043906642444980001</v>
       </c>
       <c r="B136" s="0">
-        <v>0.00034357206672406372</v>
+        <v>0.000369224839140243</v>
       </c>
       <c r="C136" s="0">
-        <v>0.00028577342983141126</v>
+        <v>0.00028399037593870429</v>
       </c>
       <c r="D136" s="0">
-        <v>0.00030739</v>
+        <v>0.0002682960254925065</v>
       </c>
       <c r="E136" s="0">
-        <v>0.00015743501598607446</v>
+        <v>0.00012466488309945768</v>
       </c>
       <c r="F136" s="0">
-        <v>0.00011956667471726626</v>
+        <v>0.00013124104157298508</v>
       </c>
       <c r="G136" s="0">
-        <v>6.9159639995952087e-07</v>
+        <v>4.75704583820791e-05</v>
       </c>
       <c r="H136" s="0">
-        <v>21.100000000000001</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0">
-        <v>0.00040361689607648296</v>
+        <v>0.00038402519680820333</v>
       </c>
       <c r="B137" s="0">
-        <v>0.00042464576502440464</v>
+        <v>0.00036105362436129884</v>
       </c>
       <c r="C137" s="0">
-        <v>0.0002956663613593573</v>
+        <v>0.0003095017011928424</v>
       </c>
       <c r="D137" s="0">
-        <v>0.00024159210081356699</v>
+        <v>0.00025318300583717491</v>
       </c>
       <c r="E137" s="0">
-        <v>0.00018544957728718945</v>
+        <v>0.00011626886522113824</v>
       </c>
       <c r="F137" s="0">
-        <v>0.00012018742877616202</v>
+        <v>0.00011888915854291601</v>
       </c>
       <c r="G137" s="0">
-        <v>9.725499999999999e-07</v>
+        <v>4.9784093014803775e-05</v>
       </c>
       <c r="H137" s="0">
-        <v>21.199999999999999</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0">
-        <v>0.0003809660629158037</v>
+        <v>0.00040555333222701571</v>
       </c>
       <c r="B138" s="0">
-        <v>0.00035087026423925172</v>
+        <v>0.00033654700728666761</v>
       </c>
       <c r="C138" s="0">
-        <v>0.00029326027649308325</v>
+        <v>0.000305694105804182</v>
       </c>
       <c r="D138" s="0">
-        <v>0.00028618686855615854</v>
+        <v>0.00022909701425347635</v>
       </c>
       <c r="E138" s="0">
-        <v>0.00015722776997318088</v>
+        <v>0.00011127295028662013</v>
       </c>
       <c r="F138" s="0">
-        <v>0.00012195751661074543</v>
+        <v>0.00013887094757879861</v>
       </c>
       <c r="G138" s="0">
-        <v>4.7116345977890171e-06</v>
+        <v>4.7494739835077265e-05</v>
       </c>
       <c r="H138" s="0">
-        <v>21.300000000000001</v>
+        <v>13.699999999999999</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0">
-        <v>0.00041035747155033239</v>
+        <v>0.00038955165529075419</v>
       </c>
       <c r="B139" s="0">
-        <v>0.00042448388123875755</v>
+        <v>0.00037745870858322297</v>
       </c>
       <c r="C139" s="0">
-        <v>0.00028707223020498163</v>
+        <v>0.00036025</v>
       </c>
       <c r="D139" s="0">
-        <v>0.00024171529659168208</v>
+        <v>0.00024161353150512106</v>
       </c>
       <c r="E139" s="0">
-        <v>0.00017383658756468307</v>
+        <v>0.00010651703289946962</v>
       </c>
       <c r="F139" s="0">
-        <v>0.00012448773544132324</v>
+        <v>0.00011706062302625645</v>
       </c>
       <c r="G139" s="0">
-        <v>8.430192142771746e-06</v>
+        <v>5.0523312282505353e-05</v>
       </c>
       <c r="H139" s="0">
-        <v>21.399999999999999</v>
+        <v>13.800000000000001</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0">
-        <v>0.00038319494903305099</v>
+        <v>0.00039061937326962331</v>
       </c>
       <c r="B140" s="0">
-        <v>0.0003593751449620789</v>
+        <v>0.00033128040389948806</v>
       </c>
       <c r="C140" s="0">
-        <v>0.00030753489284978986</v>
+        <v>0.00029185024713997994</v>
       </c>
       <c r="D140" s="0">
-        <v>0.00027074786559491768</v>
+        <v>0.00024062758655448747</v>
       </c>
       <c r="E140" s="0">
-        <v>0.00016051914483186972</v>
+        <v>9.9795177362592497e-05</v>
       </c>
       <c r="F140" s="0">
-        <v>0.00013222268156095837</v>
+        <v>0.00014753124483640607</v>
       </c>
       <c r="G140" s="0">
-        <v>1.2600715313424414e-05</v>
+        <v>4.7609679903952967e-05</v>
       </c>
       <c r="H140" s="0">
-        <v>21.5</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0">
-        <v>0.00041764326938574698</v>
+        <v>0.00039777007489637782</v>
       </c>
       <c r="B141" s="0">
-        <v>0.00039820064724569696</v>
+        <v>0.00039823959246943082</v>
       </c>
       <c r="C141" s="0">
-        <v>0.00028313476522883293</v>
+        <v>0.00031094959737385083</v>
       </c>
       <c r="D141" s="0">
-        <v>0.00024583944851884232</v>
+        <v>0.00023554065010837378</v>
       </c>
       <c r="E141" s="0">
-        <v>0.00016558538425519794</v>
+        <v>9.7292139985956098e-05</v>
       </c>
       <c r="F141" s="0">
-        <v>0.00013085054366301249</v>
+        <v>0.00011914631128165812</v>
       </c>
       <c r="G141" s="0">
-        <v>1.5168913096303569e-05</v>
+        <v>5.1541726706787526e-05</v>
       </c>
       <c r="H141" s="0">
-        <v>21.600000000000001</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0">
-        <v>0.00038635419994989138</v>
+        <v>0.00038292617022614721</v>
       </c>
       <c r="B142" s="0">
-        <v>0.0003690735522066414</v>
+        <v>0.00033239922309838898</v>
       </c>
       <c r="C142" s="0">
-        <v>0.00033218613670190874</v>
+        <v>0.0002845041838843538</v>
       </c>
       <c r="D142" s="0">
-        <v>0.0002600973316340633</v>
+        <v>0.00025803109575709825</v>
       </c>
       <c r="E142" s="0">
-        <v>0.0001676841002176234</v>
+        <v>9.1545023170661006e-05</v>
       </c>
       <c r="F142" s="0">
-        <v>0.00014422095733116416</v>
+        <v>0.00013228364155610373</v>
       </c>
       <c r="G142" s="0">
-        <v>1.9473161581188467e-05</v>
+        <v>4.7812975648169164e-05</v>
       </c>
       <c r="H142" s="0">
-        <v>21.699999999999999</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0">
-        <v>0.00042570267560940335</v>
+        <v>0.0004071413050104516</v>
       </c>
       <c r="B143" s="0">
-        <v>0.00038497430027418052</v>
+        <v>0.00042483000000000001</v>
       </c>
       <c r="C143" s="0">
-        <v>0.00028249763809656424</v>
+        <v>0.00028997165406540295</v>
       </c>
       <c r="D143" s="0">
-        <v>0.00025600024462552582</v>
+        <v>0.00023444050291918482</v>
       </c>
       <c r="E143" s="0">
-        <v>0.00016021270751400584</v>
+        <v>8.9190440773845921e-05</v>
       </c>
       <c r="F143" s="0">
-        <v>0.00013980811335005265</v>
+        <v>0.00013005032742232712</v>
       </c>
       <c r="G143" s="0">
-        <v>2.1558839395057611e-05</v>
+        <v>5.2955947933293523e-05</v>
       </c>
       <c r="H143" s="0">
-        <v>21.800000000000001</v>
+        <v>14.199999999999999</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0">
-        <v>0.00039023478888633022</v>
+        <v>0.00038004847928442299</v>
       </c>
       <c r="B144" s="0">
-        <v>0.00038020383533981958</v>
+        <v>0.00033769805734121662</v>
       </c>
       <c r="C144" s="0">
-        <v>0.00035023304669740395</v>
+        <v>0.00028251686361306563</v>
       </c>
       <c r="D144" s="0">
-        <v>0.0002516478799932222</v>
+        <v>0.00028158636956344854</v>
       </c>
       <c r="E144" s="0">
-        <v>0.00017680605361869182</v>
+        <v>8.9660999999999994e-05</v>
       </c>
       <c r="F144" s="0">
-        <v>0.00012721930476823086</v>
+        <v>0.00012212015561938622</v>
       </c>
       <c r="G144" s="0">
-        <v>2.4767148855892695e-05</v>
+        <v>4.8234229267134119e-05</v>
       </c>
       <c r="H144" s="0">
-        <v>21.899999999999999</v>
+        <v>14.300000000000001</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0">
+        <v>0.00041797542280046251</v>
+      </c>
+      <c r="B145" s="0">
+        <v>0.00039845555352350007</v>
+      </c>
+      <c r="C145" s="0">
+        <v>0.00028264859761394291</v>
+      </c>
+      <c r="D145" s="0">
+        <v>0.00024049864217464838</v>
+      </c>
+      <c r="E145" s="0">
+        <v>7.1464739339885137e-05</v>
+      </c>
+      <c r="F145" s="0">
+        <v>0.00011581129709549855</v>
+      </c>
+      <c r="G145" s="0">
+        <v>4.8039110112121988e-05</v>
+      </c>
+      <c r="H145" s="0">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="0">
+        <v>0.00038044931509103984</v>
+      </c>
+      <c r="B146" s="0">
+        <v>0.00034700009530561499</v>
+      </c>
+      <c r="C146" s="0">
+        <v>0.00028812512079908647</v>
+      </c>
+      <c r="D146" s="0">
+        <v>0.00030191207923743236</v>
+      </c>
+      <c r="E146" s="0">
+        <v>5.7230715074354173e-05</v>
+      </c>
+      <c r="F146" s="0">
+        <v>0.00011422071878915152</v>
+      </c>
+      <c r="G146" s="0">
+        <v>4.8804652650245278e-05</v>
+      </c>
+      <c r="H146" s="0">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="0">
+        <v>0.00043040018860040076</v>
+      </c>
+      <c r="B147" s="0">
+        <v>0.00037928523459985174</v>
+      </c>
+      <c r="C147" s="0">
+        <v>0.00028275382141413502</v>
+      </c>
+      <c r="D147" s="0">
+        <v>0.0002601110443818736</v>
+      </c>
+      <c r="E147" s="0">
+        <v>4.7783420543903683e-05</v>
+      </c>
+      <c r="F147" s="0">
+        <v>0.0001181678891230736</v>
+      </c>
+      <c r="G147" s="0">
+        <v>4.7597196691758772e-05</v>
+      </c>
+      <c r="H147" s="0">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="0">
+        <v>0.00038327374249419438</v>
+      </c>
+      <c r="B148" s="0">
+        <v>0.00035890137226890105</v>
+      </c>
+      <c r="C148" s="0">
+        <v>0.00030593538893051704</v>
+      </c>
+      <c r="D148" s="0">
+        <v>0.00026837013312923684</v>
+      </c>
+      <c r="E148" s="0">
+        <v>3.5983012152438639e-05</v>
+      </c>
+      <c r="F148" s="0">
+        <v>0.00010824649821246529</v>
+      </c>
+      <c r="G148" s="0">
+        <v>4.9913236920845194e-05</v>
+      </c>
+      <c r="H148" s="0">
+        <v>14.699999999999999</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0">
+        <v>0.00044438708990605881</v>
+      </c>
+      <c r="B149" s="0">
+        <v>0.0003643330175526528</v>
+      </c>
+      <c r="C149" s="0">
+        <v>0.0002874768797018739</v>
+      </c>
+      <c r="D149" s="0">
+        <v>0.00030383</v>
+      </c>
+      <c r="E149" s="0">
+        <v>2.436635209399672e-05</v>
+      </c>
+      <c r="F149" s="0">
+        <v>0.00012215080443482362</v>
+      </c>
+      <c r="G149" s="0">
+        <v>4.7430923209598353e-05</v>
+      </c>
+      <c r="H149" s="0">
+        <v>14.800000000000001</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="0">
+        <v>0.00038803136757085022</v>
+      </c>
+      <c r="B150" s="0">
+        <v>0.0003734099484722389</v>
+      </c>
+      <c r="C150" s="0">
+        <v>0.00034540699839288169</v>
+      </c>
+      <c r="D150" s="0">
+        <v>0.00025375104215036434</v>
+      </c>
+      <c r="E150" s="0">
+        <v>1.5920576453882631e-05</v>
+      </c>
+      <c r="F150" s="0">
+        <v>0.00010489689710879024</v>
+      </c>
+      <c r="G150" s="0">
+        <v>5.0833326010210756e-05</v>
+      </c>
+      <c r="H150" s="0">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="0">
+        <v>0.00038911758506624601</v>
+      </c>
+      <c r="B151" s="0">
+        <v>0.00033121320525012616</v>
+      </c>
+      <c r="C151" s="0">
+        <v>0.00029153414395303924</v>
+      </c>
+      <c r="D151" s="0">
+        <v>0.0002502800596846205</v>
+      </c>
+      <c r="E151" s="0">
+        <v>5.7826935729805064e-06</v>
+      </c>
+      <c r="F151" s="0">
+        <v>0.00012930026684606759</v>
+      </c>
+      <c r="G151" s="0">
+        <v>4.7484201890538678e-05</v>
+      </c>
+      <c r="H151" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="0">
+        <v>0.0003950736001928272</v>
+      </c>
+      <c r="B152" s="0">
+        <v>0.00039113422011203099</v>
+      </c>
+      <c r="C152" s="0">
+        <v>0.00032269957864226244</v>
+      </c>
+      <c r="D152" s="0">
+        <v>0.00024440324350237785</v>
+      </c>
+      <c r="E152" s="0">
+        <v>2.5506964967414554e-06</v>
+      </c>
+      <c r="F152" s="0">
+        <v>0.00010654486952733512</v>
+      </c>
+      <c r="G152" s="0">
+        <v>5.2158275414052578e-05</v>
+      </c>
+      <c r="H152" s="0">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="0">
+        <v>0.00038258174766707062</v>
+      </c>
+      <c r="B153" s="0">
+        <v>0.00033268659361531777</v>
+      </c>
+      <c r="C153" s="0">
+        <v>0.00028471323236037033</v>
+      </c>
+      <c r="D153" s="0">
+        <v>0.00026569964599024973</v>
+      </c>
+      <c r="E153" s="0">
+        <v>2.915e-06</v>
+      </c>
+      <c r="F153" s="0">
+        <v>0.00011248981646144908</v>
+      </c>
+      <c r="G153" s="0">
+        <v>4.7720787633420613e-05</v>
+      </c>
+      <c r="H153" s="0">
+        <v>15.199999999999999</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="0">
+        <v>0.00040337715005314901</v>
+      </c>
+      <c r="B154" s="0">
+        <v>0.00042492442561502692</v>
+      </c>
+      <c r="C154" s="0">
+        <v>0.00029643586174660696</v>
+      </c>
+      <c r="D154" s="0">
+        <v>0.00024004866263858769</v>
+      </c>
+      <c r="E154" s="0">
+        <v>1.4147627220485811e-05</v>
+      </c>
+      <c r="F154" s="0">
+        <v>0.00011733532179885942</v>
+      </c>
+      <c r="G154" s="0">
+        <v>5.3743280018069221e-05</v>
+      </c>
+      <c r="H154" s="0">
+        <v>15.300000000000001</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="0">
+        <v>0.00038001783279442052</v>
+      </c>
+      <c r="B155" s="0">
+        <v>0.00033772206696164791</v>
+      </c>
+      <c r="C155" s="0">
+        <v>0.00028296368922259941</v>
+      </c>
+      <c r="D155" s="0">
+        <v>0.00028665984268511953</v>
+      </c>
+      <c r="E155" s="0">
+        <v>2.5396156858857573e-05</v>
+      </c>
+      <c r="F155" s="0">
+        <v>9.8538287937354133e-05</v>
+      </c>
+      <c r="G155" s="0">
+        <v>4.8115797852195453e-05</v>
+      </c>
+      <c r="H155" s="0">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="0">
+        <v>0.00041282245142426448</v>
+      </c>
+      <c r="B156" s="0">
+        <v>0.0004247108524774</v>
+      </c>
+      <c r="C156" s="0">
+        <v>0.00028531790616363647</v>
+      </c>
+      <c r="D156" s="0">
+        <v>0.00024072748845811756</v>
+      </c>
+      <c r="E156" s="0">
+        <v>3.874493694021635e-05</v>
+      </c>
+      <c r="F156" s="0">
+        <v>9.2531795503955107e-05</v>
+      </c>
+      <c r="G156" s="0">
+        <v>5.5801563190681004e-05</v>
+      </c>
+      <c r="H156" s="0">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="0">
+        <v>0.00038030087135258809</v>
+      </c>
+      <c r="B157" s="0">
+        <v>0.00034622768957102903</v>
+      </c>
+      <c r="C157" s="0">
+        <v>0.00028782067206969047</v>
+      </c>
+      <c r="D157" s="0">
+        <v>0.00030604799055154356</v>
+      </c>
+      <c r="E157" s="0">
+        <v>4.6667195989291059e-05</v>
+      </c>
+      <c r="F157" s="0">
+        <v>8.6045806593740225e-05</v>
+      </c>
+      <c r="G157" s="0">
+        <v>4.9033569128791386e-05</v>
+      </c>
+      <c r="H157" s="0">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="0">
+        <v>0.0004234622523383356</v>
+      </c>
+      <c r="B158" s="0">
+        <v>0.00038902069413741461</v>
+      </c>
+      <c r="C158" s="0">
+        <v>0.00028236378898102276</v>
+      </c>
+      <c r="D158" s="0">
+        <v>0.00025009885961983812</v>
+      </c>
+      <c r="E158" s="0">
+        <v>6.0169947001679595e-05</v>
+      </c>
+      <c r="F158" s="0">
+        <v>8.3573443346892734e-05</v>
+      </c>
+      <c r="G158" s="0">
+        <v>4.7651781725268361e-05</v>
+      </c>
+      <c r="H158" s="0">
+        <v>15.699999999999999</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="0">
+        <v>0.0003826983855603393</v>
+      </c>
+      <c r="B159" s="0">
+        <v>0.00035705277158946757</v>
+      </c>
+      <c r="C159" s="0">
+        <v>0.00030255711354879337</v>
+      </c>
+      <c r="D159" s="0">
+        <v>0.00027442745290771821</v>
+      </c>
+      <c r="E159" s="0">
+        <v>6.7142432427889451e-05</v>
+      </c>
+      <c r="F159" s="0">
+        <v>7.5439152419880273e-05</v>
+      </c>
+      <c r="G159" s="0">
+        <v>4.9936917744520296e-05</v>
+      </c>
+      <c r="H159" s="0">
+        <v>15.800000000000001</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="0">
+        <v>0.00043545759531901895</v>
+      </c>
+      <c r="B160" s="0">
+        <v>0.000373153835726676</v>
+      </c>
+      <c r="C160" s="0">
+        <v>0.00028440061005408773</v>
+      </c>
+      <c r="D160" s="0">
+        <v>0.00027508918319852694</v>
+      </c>
+      <c r="E160" s="0">
+        <v>7.6369673816127826e-05</v>
+      </c>
+      <c r="F160" s="0">
+        <v>7.8093046022577241e-05</v>
+      </c>
+      <c r="G160" s="0">
+        <v>4.7210575488801297e-05</v>
+      </c>
+      <c r="H160" s="0">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="0">
+        <v>0.00038688391224921321</v>
+      </c>
+      <c r="B161" s="0">
+        <v>0.00037009421809219313</v>
+      </c>
+      <c r="C161" s="0">
+        <v>0.00033461424364419646</v>
+      </c>
+      <c r="D161" s="0">
+        <v>0.00025931067456098239</v>
+      </c>
+      <c r="E161" s="0">
+        <v>8.9687116640153791e-05</v>
+      </c>
+      <c r="F161" s="0">
+        <v>6.673174521411246e-05</v>
+      </c>
+      <c r="G161" s="0">
+        <v>5.1071161137663989e-05</v>
+      </c>
+      <c r="H161" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="0">
+        <v>0.00038688391224921321</v>
+      </c>
+      <c r="B162" s="0">
+        <v>0.00037009421809219313</v>
+      </c>
+      <c r="C162" s="0">
+        <v>0.00033461424364419646</v>
+      </c>
+      <c r="D162" s="0">
+        <v>0.00025931067456098239</v>
+      </c>
+      <c r="E162" s="0">
+        <v>8.9687116640153791e-05</v>
+      </c>
+      <c r="F162" s="0">
+        <v>6.673174521411246e-05</v>
+      </c>
+      <c r="G162" s="0">
+        <v>5.1071161137663989e-05</v>
+      </c>
+      <c r="H162" s="0">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="0">
+        <v>0.00039242207617717049</v>
+      </c>
+      <c r="B163" s="0">
+        <v>0.00038571236078183743</v>
+      </c>
+      <c r="C163" s="0">
+        <v>0.00033510486668655013</v>
+      </c>
+      <c r="D163" s="0">
+        <v>0.00024880052571948311</v>
+      </c>
+      <c r="E163" s="0">
+        <v>0.00011426171484364918</v>
+      </c>
+      <c r="F163" s="0">
+        <v>6.1664881970536939e-05</v>
+      </c>
+      <c r="G163" s="0">
+        <v>5.2701755032791614e-05</v>
+      </c>
+      <c r="H163" s="0">
+        <v>16.199999999999999</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="0">
+        <v>0.00040023167553842947</v>
+      </c>
+      <c r="B164" s="0">
+        <v>0.00040517558439455838</v>
+      </c>
+      <c r="C164" s="0">
+        <v>0.00030369318661145953</v>
+      </c>
+      <c r="D164" s="0">
+        <v>0.00024251784691375284</v>
+      </c>
+      <c r="E164" s="0">
+        <v>0.00014061754015194525</v>
+      </c>
+      <c r="F164" s="0">
+        <v>4.4427585611401548e-05</v>
+      </c>
+      <c r="G164" s="0">
+        <v>5.4691588460083642e-05</v>
+      </c>
+      <c r="H164" s="0">
+        <v>16.300000000000001</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="0">
+        <v>0.00040022927225857034</v>
+      </c>
+      <c r="B165" s="0">
+        <v>0.00040517558439455838</v>
+      </c>
+      <c r="C165" s="0">
+        <v>0.00030369318661145953</v>
+      </c>
+      <c r="D165" s="0">
+        <v>0.00024251784691375284</v>
+      </c>
+      <c r="E165" s="0">
+        <v>0.00014061754015194525</v>
+      </c>
+      <c r="F165" s="0">
+        <v>4.4427585611401548e-05</v>
+      </c>
+      <c r="G165" s="0">
+        <v>5.4691588460083642e-05</v>
+      </c>
+      <c r="H165" s="0">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="0">
+        <v>0.00037998124022762489</v>
+      </c>
+      <c r="B166" s="0">
+        <v>0.00033771222765599778</v>
+      </c>
+      <c r="C166" s="0">
+        <v>0.00028309144425712161</v>
+      </c>
+      <c r="D166" s="0">
+        <v>0.00028785854783422524</v>
+      </c>
+      <c r="E166" s="0">
+        <v>0.00012038627853673839</v>
+      </c>
+      <c r="F166" s="0">
+        <v>3.6170716177013121e-05</v>
+      </c>
+      <c r="G166" s="0">
+        <v>4.7738610965053868e-05</v>
+      </c>
+      <c r="H166" s="0">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="0">
+        <v>0.000408520798342494</v>
+      </c>
+      <c r="B167" s="0">
+        <v>0.00042477079236374231</v>
+      </c>
+      <c r="C167" s="0">
+        <v>0.00028899401088924561</v>
+      </c>
+      <c r="D167" s="0">
+        <v>0.00024096738497438069</v>
+      </c>
+      <c r="E167" s="0">
+        <v>0.00013534433620406824</v>
+      </c>
+      <c r="F167" s="0">
+        <v>2.7019873938729639e-05</v>
+      </c>
+      <c r="G167" s="0">
+        <v>5.8781816239861554e-05</v>
+      </c>
+      <c r="H167" s="0">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="0">
+        <v>0.00038012313511636255</v>
+      </c>
+      <c r="B168" s="0">
+        <v>0.0003455682805653576</v>
+      </c>
+      <c r="C168" s="0">
+        <v>0.00028726977464685517</v>
+      </c>
+      <c r="D168" s="0">
+        <v>0.00030702532258611694</v>
+      </c>
+      <c r="E168" s="0">
+        <v>0.00012358744954072553</v>
+      </c>
+      <c r="F168" s="0">
+        <v>1.8240220569684677e-05</v>
+      </c>
+      <c r="G168" s="0">
+        <v>4.868359933835818e-05</v>
+      </c>
+      <c r="H168" s="0">
+        <v>16.699999999999999</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="0">
+        <v>0.00041788323518834658</v>
+      </c>
+      <c r="B169" s="0">
+        <v>0.00039843675531230332</v>
+      </c>
+      <c r="C169" s="0">
+        <v>0.00028318601863142073</v>
+      </c>
+      <c r="D169" s="0">
+        <v>0.00024552171554508679</v>
+      </c>
+      <c r="E169" s="0">
+        <v>0.00013467885322953032</v>
+      </c>
+      <c r="F169" s="0">
+        <v>1.1806501046496648e-05</v>
+      </c>
+      <c r="G169" s="0">
+        <v>5.6202620232903484e-05</v>
+      </c>
+      <c r="H169" s="0">
+        <v>16.800000000000001</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="0">
+        <v>0.00038222002317662702</v>
+      </c>
+      <c r="B170" s="0">
+        <v>0.00035543315674260056</v>
+      </c>
+      <c r="C170" s="0">
+        <v>0.0003000289389807318</v>
+      </c>
+      <c r="D170" s="0">
+        <v>0.00027681407726083782</v>
+      </c>
+      <c r="E170" s="0">
+        <v>0.0001322300231104163</v>
+      </c>
+      <c r="F170" s="0">
+        <v>4.27903096474117e-06</v>
+      </c>
+      <c r="G170" s="0">
+        <v>4.972759675914818e-05</v>
+      </c>
+      <c r="H170" s="0">
+        <v>16.899999999999999</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="0">
+        <v>0.00042833731321627571</v>
+      </c>
+      <c r="B171" s="0">
+        <v>0.00038181484291667256</v>
+      </c>
+      <c r="C171" s="0">
+        <v>0.00028284130868026054</v>
+      </c>
+      <c r="D171" s="0">
+        <v>0.00025962142649091049</v>
+      </c>
+      <c r="E171" s="0">
+        <v>0.00013621880155562498</v>
+      </c>
+      <c r="F171" s="0">
+        <v>1.9592863345467642e-06</v>
+      </c>
+      <c r="G171" s="0">
+        <v>4.6666521757141036e-05</v>
+      </c>
+      <c r="H171" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="0">
+        <v>0.00038591223487670589</v>
+      </c>
+      <c r="B172" s="0">
+        <v>0.00036716527558118453</v>
+      </c>
+      <c r="C172" s="0">
+        <v>0.00032616348311325359</v>
+      </c>
+      <c r="D172" s="0">
+        <v>0.0002623106954531898</v>
+      </c>
+      <c r="E172" s="0">
+        <v>0.00014451653770263174</v>
+      </c>
+      <c r="F172" s="0">
+        <v>2.2769000000000002e-06</v>
+      </c>
+      <c r="G172" s="0">
+        <v>5.1002836254218193e-05</v>
+      </c>
+      <c r="H172" s="0">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="0">
+        <v>0.00044002285932271361</v>
+      </c>
+      <c r="B173" s="0">
+        <v>0.00036825580400327303</v>
+      </c>
+      <c r="C173" s="0">
+        <v>0.00028608485420510192</v>
+      </c>
+      <c r="D173" s="0">
+        <v>0.0002915875372434728</v>
+      </c>
+      <c r="E173" s="0">
+        <v>0.00013940167853789288</v>
+      </c>
+      <c r="F173" s="0">
+        <v>1.1040022555799745e-05</v>
+      </c>
+      <c r="G173" s="0">
+        <v>4.6308226026315331e-05</v>
+      </c>
+      <c r="H173" s="0">
+        <v>17.199999999999999</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="0">
+        <v>0.00039080106547084118</v>
+      </c>
+      <c r="B174" s="0">
+        <v>0.00038113498931469081</v>
+      </c>
+      <c r="C174" s="0">
+        <v>0.00034799075762492206</v>
+      </c>
+      <c r="D174" s="0">
+        <v>0.00025057143675231649</v>
+      </c>
+      <c r="E174" s="0">
+        <v>0.00016047691228825733</v>
+      </c>
+      <c r="F174" s="0">
+        <v>1.9800431785027068e-05</v>
+      </c>
+      <c r="G174" s="0">
+        <v>5.2867813677909956e-05</v>
+      </c>
+      <c r="H174" s="0">
+        <v>17.300000000000001</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="0">
+        <v>0.00038198822926611769</v>
+      </c>
+      <c r="B175" s="0">
+        <v>0.00033313851576276482</v>
+      </c>
+      <c r="C175" s="0">
+        <v>0.00028438814160239019</v>
+      </c>
+      <c r="D175" s="0">
+        <v>0.00026923994381984612</v>
+      </c>
+      <c r="E175" s="0">
+        <v>0.0001761664516706667</v>
+      </c>
+      <c r="F175" s="0">
+        <v>2.9692297266431912e-05</v>
+      </c>
+      <c r="G175" s="0">
+        <v>4.6229013775915373e-05</v>
+      </c>
+      <c r="H175" s="0">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="0">
+        <v>0.00039764224848402635</v>
+      </c>
+      <c r="B176" s="0">
+        <v>0.00039820044883489051</v>
+      </c>
+      <c r="C176" s="0">
+        <v>0.0003118582113779634</v>
+      </c>
+      <c r="D176" s="0">
+        <v>0.00024419844086275287</v>
+      </c>
+      <c r="E176" s="0">
+        <v>0.00018468220887424766</v>
+      </c>
+      <c r="F176" s="0">
+        <v>3.61556912088641e-05</v>
+      </c>
+      <c r="G176" s="0">
+        <v>5.5366134902624565e-05</v>
+      </c>
+      <c r="H176" s="0">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="0">
+        <v>0.00037993347909739408</v>
+      </c>
+      <c r="B177" s="0">
+        <v>0.00033768649103479065</v>
+      </c>
+      <c r="C177" s="0">
+        <v>0.00028312687728656671</v>
+      </c>
+      <c r="D177" s="0">
+        <v>0.00028817116701112123</v>
+      </c>
+      <c r="E177" s="0">
+        <v>0.00015311354507898463</v>
+      </c>
+      <c r="F177" s="0">
+        <v>4.6072236837744419e-05</v>
+      </c>
+      <c r="G177" s="0">
+        <v>4.6409412132315982e-05</v>
+      </c>
+      <c r="H177" s="0">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="0">
+        <v>0.00040504768426313624</v>
+      </c>
+      <c r="B178" s="0">
+        <v>0.00042480834862294317</v>
+      </c>
+      <c r="C178" s="0">
+        <v>0.00029345968312478405</v>
+      </c>
+      <c r="D178" s="0">
+        <v>0.00024120030861736914</v>
+      </c>
+      <c r="E178" s="0">
+        <v>0.00017257020210852863</v>
+      </c>
+      <c r="F178" s="0">
+        <v>5.1728910279243892e-05</v>
+      </c>
+      <c r="G178" s="0">
+        <v>5.5124037997139461e-05</v>
+      </c>
+      <c r="H178" s="0">
+        <v>17.699999999999999</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="0">
+        <v>0.00038003652796658716</v>
+      </c>
+      <c r="B179" s="0">
+        <v>0.00034493695783200892</v>
+      </c>
+      <c r="C179" s="0">
+        <v>0.00028689680552876893</v>
+      </c>
+      <c r="D179" s="0">
+        <v>0.00030729227627228529</v>
+      </c>
+      <c r="E179" s="0">
+        <v>0.00014868484003647373</v>
+      </c>
+      <c r="F179" s="0">
+        <v>5.8903445315157838e-05</v>
+      </c>
+      <c r="G179" s="0">
+        <v>4.7154673115821121e-05</v>
+      </c>
+      <c r="H179" s="0">
+        <v>17.800000000000001</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="0">
+        <v>0.00041330771789193065</v>
+      </c>
+      <c r="B180" s="0">
+        <v>0.00042461312441970941</v>
+      </c>
+      <c r="C180" s="0">
+        <v>0.00028507299108129216</v>
+      </c>
+      <c r="D180" s="0">
+        <v>0.00024260464060025077</v>
+      </c>
+      <c r="E180" s="0">
+        <v>0.00016267369469667053</v>
+      </c>
+      <c r="F180" s="0">
+        <v>6.8793818410534807e-05</v>
+      </c>
+      <c r="G180" s="0">
+        <v>5.1349631223853473e-05</v>
+      </c>
+      <c r="H180" s="0">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="0">
+        <v>0.00042263658554286913</v>
+      </c>
+      <c r="B181" s="0">
+        <v>0.00039022460742583592</v>
+      </c>
+      <c r="C181" s="0">
+        <v>0.0002824991476365973</v>
+      </c>
+      <c r="D181" s="0">
+        <v>0.00025123454853737641</v>
+      </c>
+      <c r="E181" s="0">
+        <v>0.00015649654231147101</v>
+      </c>
+      <c r="F181" s="0">
+        <v>8.6109326009228211e-05</v>
+      </c>
+      <c r="G181" s="0">
+        <v>4.4668336411425145e-05</v>
+      </c>
+      <c r="H181" s="0">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="0">
+        <v>0.00038507274854935063</v>
+      </c>
+      <c r="B182" s="0">
+        <v>0.00036483926768487594</v>
+      </c>
+      <c r="C182" s="0">
+        <v>0.00031992875715390091</v>
+      </c>
+      <c r="D182" s="0">
+        <v>0.00026506155257288694</v>
+      </c>
+      <c r="E182" s="0">
+        <v>0.0001591575848330936</v>
+      </c>
+      <c r="F182" s="0">
+        <v>9.78150678888276e-05</v>
+      </c>
+      <c r="G182" s="0">
+        <v>4.9136529576521611e-05</v>
+      </c>
+      <c r="H182" s="0">
+        <v>18.199999999999999</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="0">
+        <v>0.0004327808641336705</v>
+      </c>
+      <c r="B183" s="0">
+        <v>0.0003758961980946703</v>
+      </c>
+      <c r="C183" s="0">
+        <v>0.00028380656905634393</v>
+      </c>
+      <c r="D183" s="0">
+        <v>0.00026968978035771517</v>
+      </c>
+      <c r="E183" s="0">
+        <v>0.00015331144650088585</v>
+      </c>
+      <c r="F183" s="0">
+        <v>0.0001087361715420914</v>
+      </c>
+      <c r="G183" s="0">
+        <v>4.3458412126515643e-05</v>
+      </c>
+      <c r="H183" s="0">
+        <v>18.300000000000001</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="0">
+        <v>0.00038938738530532144</v>
+      </c>
+      <c r="B184" s="0">
+        <v>0.00037742531329545569</v>
+      </c>
+      <c r="C184" s="0">
+        <v>0.00036146000000000003</v>
+      </c>
+      <c r="D184" s="0">
+        <v>0.00025353881884849821</v>
+      </c>
+      <c r="E184" s="0">
+        <v>0.000169765067159418</v>
+      </c>
+      <c r="F184" s="0">
+        <v>9.6568531907344939e-05</v>
+      </c>
+      <c r="G184" s="0">
+        <v>5.1150164233478986e-05</v>
+      </c>
+      <c r="H184" s="0">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="0">
+        <v>0.00044421328440124344</v>
+      </c>
+      <c r="B185" s="0">
+        <v>0.0003642544185057215</v>
+      </c>
+      <c r="C185" s="0">
+        <v>0.00028782486224797951</v>
+      </c>
+      <c r="D185" s="0">
+        <v>0.00030739999999999999</v>
+      </c>
+      <c r="E185" s="0">
+        <v>0.0001540231045654136</v>
+      </c>
+      <c r="F185" s="0">
+        <v>0.00010757903629168223</v>
+      </c>
+      <c r="G185" s="0">
+        <v>4.2544425759221937e-05</v>
+      </c>
+      <c r="H185" s="0">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="0">
+        <v>0.000395478019881029</v>
+      </c>
+      <c r="B186" s="0">
+        <v>0.00039237312034107684</v>
+      </c>
+      <c r="C186" s="0">
+        <v>0.00032062359078040476</v>
+      </c>
+      <c r="D186" s="0">
+        <v>0.00024596695212480594</v>
+      </c>
+      <c r="E186" s="0">
+        <v>0.00018491724810573763</v>
+      </c>
+      <c r="F186" s="0">
+        <v>9.6163265471782165e-05</v>
+      </c>
+      <c r="G186" s="0">
+        <v>5.2483345942018852e-05</v>
+      </c>
+      <c r="H186" s="0">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="0">
+        <v>0.00037988763299700456</v>
+      </c>
+      <c r="B187" s="0">
+        <v>0.00033764902196670046</v>
+      </c>
+      <c r="C187" s="0">
+        <v>0.0002831291216530299</v>
+      </c>
+      <c r="D187" s="0">
+        <v>0.00028825940875697485</v>
+      </c>
+      <c r="E187" s="0">
+        <v>0.00016141810289328301</v>
+      </c>
+      <c r="F187" s="0">
+        <v>0.00010083520724207844</v>
+      </c>
+      <c r="G187" s="0">
+        <v>4.1923998804146153e-05</v>
+      </c>
+      <c r="H187" s="0">
+        <v>18.699999999999999</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="0">
+        <v>0.00040208612668883972</v>
+      </c>
+      <c r="B188" s="0">
+        <v>0.00042482068432186606</v>
+      </c>
+      <c r="C188" s="0">
+        <v>0.00029889649533664599</v>
+      </c>
+      <c r="D188" s="0">
+        <v>0.00024201213489089728</v>
+      </c>
+      <c r="E188" s="0">
+        <v>0.00018675160468337106</v>
+      </c>
+      <c r="F188" s="0">
+        <v>0.00010102874000619502</v>
+      </c>
+      <c r="G188" s="0">
+        <v>4.6006869579689803e-05</v>
+      </c>
+      <c r="H188" s="0">
+        <v>18.800000000000001</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="0">
+        <v>0.00037988915471760571</v>
+      </c>
+      <c r="B189" s="0">
+        <v>0.00034450036034599114</v>
+      </c>
+      <c r="C189" s="0">
+        <v>0.00028649627340217283</v>
+      </c>
+      <c r="D189" s="0">
+        <v>0.00030737098996192326</v>
+      </c>
+      <c r="E189" s="0">
+        <v>0.00015511119957767403</v>
+      </c>
+      <c r="F189" s="0">
+        <v>0.00010359665977772487</v>
+      </c>
+      <c r="G189" s="0">
+        <v>4.161672214846615e-05</v>
+      </c>
+      <c r="H189" s="0">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="0">
+        <v>0.00040953265912630729</v>
+      </c>
+      <c r="B190" s="0">
+        <v>0.00042463236636216303</v>
+      </c>
+      <c r="C190" s="0">
+        <v>0.00028788027265744584</v>
+      </c>
+      <c r="D190" s="0">
+        <v>0.00024149277651625922</v>
+      </c>
+      <c r="E190" s="0">
+        <v>0.0001736803913727378</v>
+      </c>
+      <c r="F190" s="0">
+        <v>0.00010850719496213222</v>
+      </c>
+      <c r="G190" s="0">
+        <v>4.1706947000387257e-05</v>
+      </c>
+      <c r="H190" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="0">
+        <v>0.00038151463633301439</v>
+      </c>
+      <c r="B191" s="0">
+        <v>0.00035289061045873989</v>
+      </c>
+      <c r="C191" s="0">
+        <v>0.00029604826280225845</v>
+      </c>
+      <c r="D191" s="0">
+        <v>0.00028235815716253578</v>
+      </c>
+      <c r="E191" s="0">
+        <v>0.00015589537214092853</v>
+      </c>
+      <c r="F191" s="0">
+        <v>0.00011065198203045973</v>
+      </c>
+      <c r="G191" s="0">
+        <v>4.132260987058966e-05</v>
+      </c>
+      <c r="H191" s="0">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="0">
+        <v>0.0004177687477483571</v>
+      </c>
+      <c r="B192" s="0">
+        <v>0.00039832923599365545</v>
+      </c>
+      <c r="C192" s="0">
+        <v>0.00028320127519340432</v>
+      </c>
+      <c r="D192" s="0">
+        <v>0.0002458344506389971</v>
+      </c>
+      <c r="E192" s="0">
+        <v>0.00016401626080857697</v>
+      </c>
+      <c r="F192" s="0">
+        <v>0.00011891532946045304</v>
+      </c>
+      <c r="G192" s="0">
+        <v>3.7914432128473924e-05</v>
+      </c>
+      <c r="H192" s="0">
+        <v>19.199999999999999</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="0">
+        <v>0.0003843650390263374</v>
+      </c>
+      <c r="B193" s="0">
+        <v>0.00036279192915659179</v>
+      </c>
+      <c r="C193" s="0">
+        <v>0.00031505567726572263</v>
+      </c>
+      <c r="D193" s="0">
+        <v>0.00026760875237498725</v>
+      </c>
+      <c r="E193" s="0">
+        <v>0.00016127307586172047</v>
+      </c>
+      <c r="F193" s="0">
+        <v>0.00012749704438623597</v>
+      </c>
+      <c r="G193" s="0">
+        <v>4.122909806432214e-05</v>
+      </c>
+      <c r="H193" s="0">
+        <v>19.300000000000001</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="0">
+        <v>0.00042698230145499152</v>
+      </c>
+      <c r="B194" s="0">
+        <v>0.00038360380828790546</v>
+      </c>
+      <c r="C194" s="0">
+        <v>0.00028267210479419847</v>
+      </c>
+      <c r="D194" s="0">
+        <v>0.00025786451662419764</v>
+      </c>
+      <c r="E194" s="0">
+        <v>0.00015857461803323489</v>
+      </c>
+      <c r="F194" s="0">
+        <v>0.00013106221553029531</v>
+      </c>
+      <c r="G194" s="0">
+        <v>3.4659511520834067e-05</v>
+      </c>
+      <c r="H194" s="0">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="0">
+        <v>0.00038824260111763263</v>
+      </c>
+      <c r="B195" s="0">
+        <v>0.00037412402798497554</v>
+      </c>
+      <c r="C195" s="0">
+        <v>0.00034913908421271633</v>
+      </c>
+      <c r="D195" s="0">
+        <v>0.00025563690795786422</v>
+      </c>
+      <c r="E195" s="0">
+        <v>0.00017032375255516448</v>
+      </c>
+      <c r="F195" s="0">
+        <v>0.0001269646056787803</v>
+      </c>
+      <c r="G195" s="0">
+        <v>4.1314984616979181e-05</v>
+      </c>
+      <c r="H195" s="0">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="0">
+        <v>0.00043689789063666772</v>
+      </c>
+      <c r="B196" s="0">
+        <v>0.00037119469745727378</v>
+      </c>
+      <c r="C196" s="0">
+        <v>0.00028499719891668499</v>
+      </c>
+      <c r="D196" s="0">
+        <v>0.00027943614250291402</v>
+      </c>
+      <c r="E196" s="0">
+        <v>0.00015604071960330259</v>
+      </c>
+      <c r="F196" s="0">
+        <v>0.00014391932939816443</v>
+      </c>
+      <c r="G196" s="0">
+        <v>3.1747541055753856e-05</v>
+      </c>
+      <c r="H196" s="0">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="0">
+        <v>0.00039302186621724362</v>
+      </c>
+      <c r="B197" s="0">
+        <v>0.00038760809623591323</v>
+      </c>
+      <c r="C197" s="0">
+        <v>0.00032998932637252844</v>
+      </c>
+      <c r="D197" s="0">
+        <v>0.0002479592542960384</v>
+      </c>
+      <c r="E197" s="0">
+        <v>0.00018223999991138663</v>
+      </c>
+      <c r="F197" s="0">
+        <v>0.00011671766886766412</v>
+      </c>
+      <c r="G197" s="0">
+        <v>3.3955822806207834e-05</v>
+      </c>
+      <c r="H197" s="0">
+        <v>19.699999999999999</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="0">
+        <v>0.00037983548707013382</v>
+      </c>
+      <c r="B198" s="0">
+        <v>0.00033760889927089862</v>
+      </c>
+      <c r="C198" s="0">
+        <v>0.00028311314861404206</v>
+      </c>
+      <c r="D198" s="0">
+        <v>0.0002882853969048376</v>
+      </c>
+      <c r="E198" s="0">
+        <v>0.00016347221474073315</v>
+      </c>
+      <c r="F198" s="0">
+        <v>0.00011742811815592588</v>
+      </c>
+      <c r="G198" s="0">
+        <v>2.8937451254732675e-05</v>
+      </c>
+      <c r="H198" s="0">
+        <v>19.800000000000001</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="0">
+        <v>0.00039958924597638374</v>
+      </c>
+      <c r="B199" s="0">
+        <v>0.00040377288248296436</v>
+      </c>
+      <c r="C199" s="0">
+        <v>0.00030492034402949817</v>
+      </c>
+      <c r="D199" s="0">
+        <v>0.00024303134599600778</v>
+      </c>
+      <c r="E199" s="0">
+        <v>0.00019827081250733467</v>
+      </c>
+      <c r="F199" s="0">
+        <v>0.00011545632363013652</v>
+      </c>
+      <c r="G199" s="0">
+        <v>2.7963381969978955e-05</v>
+      </c>
+      <c r="H199" s="0">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="0">
+        <v>0.00037983098980074289</v>
+      </c>
+      <c r="B200" s="0">
+        <v>0.00034398992418763235</v>
+      </c>
+      <c r="C200" s="0">
+        <v>0.00028608230498257907</v>
+      </c>
+      <c r="D200" s="0">
+        <v>0.0003074004775742926</v>
+      </c>
+      <c r="E200" s="0">
+        <v>0.00015706290094026192</v>
+      </c>
+      <c r="F200" s="0">
+        <v>0.0001163716197775485</v>
+      </c>
+      <c r="G200" s="0">
+        <v>2.5848217007533918e-05</v>
+      </c>
+      <c r="H200" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="0">
+        <v>0.0004063478779601894</v>
+      </c>
+      <c r="B201" s="0">
+        <v>0.00042464983324247402</v>
+      </c>
+      <c r="C201" s="0">
+        <v>0.00029142654136816136</v>
+      </c>
+      <c r="D201" s="0">
+        <v>0.00024125164485324738</v>
+      </c>
+      <c r="E201" s="0">
+        <v>0.00018026720262323309</v>
+      </c>
+      <c r="F201" s="0">
+        <v>0.00011845174607069648</v>
+      </c>
+      <c r="G201" s="0">
+        <v>2.275058031244153e-05</v>
+      </c>
+      <c r="H201" s="0">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="0">
+        <v>0.00038120676550941756</v>
+      </c>
+      <c r="B202" s="0">
+        <v>0.00035179326377914581</v>
+      </c>
+      <c r="C202" s="0">
+        <v>0.00029452938714597578</v>
+      </c>
+      <c r="D202" s="0">
+        <v>0.00028425145520624473</v>
+      </c>
+      <c r="E202" s="0">
+        <v>0.00015697971490512307</v>
+      </c>
+      <c r="F202" s="0">
+        <v>0.00011984659736553046</v>
+      </c>
+      <c r="G202" s="0">
+        <v>2.2644821219429934e-05</v>
+      </c>
+      <c r="H202" s="0">
+        <v>20.199999999999999</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="0">
+        <v>0.00041378708156663299</v>
+      </c>
+      <c r="B203" s="0">
+        <v>0.00042448463195362987</v>
+      </c>
+      <c r="C203" s="0">
+        <v>0.00028473478194058718</v>
+      </c>
+      <c r="D203" s="0">
+        <v>0.00024319064967143702</v>
+      </c>
+      <c r="E203" s="0">
+        <v>0.00016929372878680523</v>
+      </c>
+      <c r="F203" s="0">
+        <v>0.00012460069601209908</v>
+      </c>
+      <c r="G203" s="0">
+        <v>1.824228755658202e-05</v>
+      </c>
+      <c r="H203" s="0">
+        <v>20.300000000000001</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="0">
+        <v>0.00038376282909770846</v>
+      </c>
+      <c r="B204" s="0">
+        <v>0.00036097595321465877</v>
+      </c>
+      <c r="C204" s="0">
+        <v>0.00031096640651309617</v>
+      </c>
+      <c r="D204" s="0">
+        <v>0.00026928131260034178</v>
+      </c>
+      <c r="E204" s="0">
+        <v>0.00016104794860451703</v>
+      </c>
+      <c r="F204" s="0">
+        <v>0.00013288495477084623</v>
+      </c>
+      <c r="G204" s="0">
+        <v>1.9347511244878296e-05</v>
+      </c>
+      <c r="H204" s="0">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="0">
+        <v>0.00042187544335182264</v>
+      </c>
+      <c r="B205" s="0">
+        <v>0.00039093559282772172</v>
+      </c>
+      <c r="C205" s="0">
+        <v>0.00028252524279334733</v>
+      </c>
+      <c r="D205" s="0">
+        <v>0.00024999799529348176</v>
+      </c>
+      <c r="E205" s="0">
+        <v>0.0001621066211818428</v>
+      </c>
+      <c r="F205" s="0">
+        <v>0.00013308714892742643</v>
+      </c>
+      <c r="G205" s="0">
+        <v>1.5003134306951252e-05</v>
+      </c>
+      <c r="H205" s="0">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="0">
+        <v>0.0003871828654738752</v>
+      </c>
+      <c r="B206" s="0">
+        <v>0.00037154372527705153</v>
+      </c>
+      <c r="C206" s="0">
+        <v>0.0003396030549550627</v>
+      </c>
+      <c r="D206" s="0">
+        <v>0.00025781872525527998</v>
+      </c>
+      <c r="E206" s="0">
+        <v>0.0001688210294553972</v>
+      </c>
+      <c r="F206" s="0">
+        <v>0.00013846482500039895</v>
+      </c>
+      <c r="G206" s="0">
+        <v>1.2002590161856953e-05</v>
+      </c>
+      <c r="H206" s="0">
+        <v>20.600000000000001</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="0">
+        <v>0.00043085233765042716</v>
+      </c>
+      <c r="B207" s="0">
+        <v>0.00037819065336362794</v>
+      </c>
+      <c r="C207" s="0">
+        <v>0.00028332445968963456</v>
+      </c>
+      <c r="D207" s="0">
+        <v>0.00026436500717624698</v>
+      </c>
+      <c r="E207" s="0">
+        <v>0.00015797161384160775</v>
+      </c>
+      <c r="F207" s="0">
+        <v>0.00015034149727199568</v>
+      </c>
+      <c r="G207" s="0">
+        <v>8.5612956049812498e-06</v>
+      </c>
+      <c r="H207" s="0">
+        <v>20.699999999999999</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="0">
+        <v>0.00039149361122131447</v>
+      </c>
+      <c r="B208" s="0">
+        <v>0.00038359245943870484</v>
+      </c>
+      <c r="C208" s="0">
+        <v>0.00034011643811539868</v>
+      </c>
+      <c r="D208" s="0">
+        <v>0.00024986016418736306</v>
+      </c>
+      <c r="E208" s="0">
+        <v>0.0001795921596561774</v>
+      </c>
+      <c r="F208" s="0">
+        <v>0.00012304716506929478</v>
+      </c>
+      <c r="G208" s="0">
+        <v>5.9479945467813023e-06</v>
+      </c>
+      <c r="H208" s="0">
+        <v>20.800000000000001</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="0">
+        <v>0.000440656893928742</v>
+      </c>
+      <c r="B209" s="0">
+        <v>0.00036735654284972887</v>
+      </c>
+      <c r="C209" s="0">
+        <v>0.0002863404383383508</v>
+      </c>
+      <c r="D209" s="0">
+        <v>0.00029174097821595135</v>
+      </c>
+      <c r="E209" s="0">
+        <v>0.00015675414454324827</v>
+      </c>
+      <c r="F209" s="0">
+        <v>0.00014150962254996257</v>
+      </c>
+      <c r="G209" s="0">
+        <v>3.65434697980964e-06</v>
+      </c>
+      <c r="H209" s="0">
+        <v>20.899999999999999</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="0">
+        <v>0.00039747572029880909</v>
+      </c>
+      <c r="B210" s="0">
+        <v>0.00039803527544867643</v>
+      </c>
+      <c r="C210" s="0">
+        <v>0.00031178624641719452</v>
+      </c>
+      <c r="D210" s="0">
+        <v>0.00024435826845741994</v>
+      </c>
+      <c r="E210" s="0">
+        <v>0.00019891575942469444</v>
+      </c>
+      <c r="F210" s="0">
+        <v>0.00011915207541288422</v>
+      </c>
+      <c r="G210" s="0">
+        <v>1.2581511427118601e-06</v>
+      </c>
+      <c r="H210" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="0">
+        <v>0.0003797444405846567</v>
+      </c>
+      <c r="B211" s="0">
+        <v>0.00034357206672406372</v>
+      </c>
+      <c r="C211" s="0">
+        <v>0.00028577342983141126</v>
+      </c>
+      <c r="D211" s="0">
+        <v>0.00030739</v>
+      </c>
+      <c r="E211" s="0">
+        <v>0.00015743501598607446</v>
+      </c>
+      <c r="F211" s="0">
+        <v>0.00011956667471726626</v>
+      </c>
+      <c r="G211" s="0">
+        <v>6.9159639995952087e-07</v>
+      </c>
+      <c r="H211" s="0">
+        <v>21.100000000000001</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="0">
+        <v>0.00040361689607648296</v>
+      </c>
+      <c r="B212" s="0">
+        <v>0.00042464576502440464</v>
+      </c>
+      <c r="C212" s="0">
+        <v>0.0002956663613593573</v>
+      </c>
+      <c r="D212" s="0">
+        <v>0.00024159210081356699</v>
+      </c>
+      <c r="E212" s="0">
+        <v>0.00018544957728718945</v>
+      </c>
+      <c r="F212" s="0">
+        <v>0.00012018742877616202</v>
+      </c>
+      <c r="G212" s="0">
+        <v>9.725499999999999e-07</v>
+      </c>
+      <c r="H212" s="0">
+        <v>21.199999999999999</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="0">
+        <v>0.0003809660629158037</v>
+      </c>
+      <c r="B213" s="0">
+        <v>0.00035087026423925172</v>
+      </c>
+      <c r="C213" s="0">
+        <v>0.00029326027649308325</v>
+      </c>
+      <c r="D213" s="0">
+        <v>0.00028618686855615854</v>
+      </c>
+      <c r="E213" s="0">
+        <v>0.00015722776997318088</v>
+      </c>
+      <c r="F213" s="0">
+        <v>0.00012195751661074543</v>
+      </c>
+      <c r="G213" s="0">
+        <v>4.7116345977890171e-06</v>
+      </c>
+      <c r="H213" s="0">
+        <v>21.300000000000001</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="0">
+        <v>0.00041035747155033239</v>
+      </c>
+      <c r="B214" s="0">
+        <v>0.00042448388123875755</v>
+      </c>
+      <c r="C214" s="0">
+        <v>0.00028707223020498163</v>
+      </c>
+      <c r="D214" s="0">
+        <v>0.00024171529659168208</v>
+      </c>
+      <c r="E214" s="0">
+        <v>0.00017383658756468307</v>
+      </c>
+      <c r="F214" s="0">
+        <v>0.00012448773544132324</v>
+      </c>
+      <c r="G214" s="0">
+        <v>8.430192142771746e-06</v>
+      </c>
+      <c r="H214" s="0">
+        <v>21.399999999999999</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="0">
+        <v>0.00038319494903305099</v>
+      </c>
+      <c r="B215" s="0">
+        <v>0.0003593751449620789</v>
+      </c>
+      <c r="C215" s="0">
+        <v>0.00030753489284978986</v>
+      </c>
+      <c r="D215" s="0">
+        <v>0.00027074786559491768</v>
+      </c>
+      <c r="E215" s="0">
+        <v>0.00016051914483186972</v>
+      </c>
+      <c r="F215" s="0">
+        <v>0.00013222268156095837</v>
+      </c>
+      <c r="G215" s="0">
+        <v>1.2600715313424414e-05</v>
+      </c>
+      <c r="H215" s="0">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="0">
+        <v>0.00041764326938574698</v>
+      </c>
+      <c r="B216" s="0">
+        <v>0.00039820064724569696</v>
+      </c>
+      <c r="C216" s="0">
+        <v>0.00028313476522883293</v>
+      </c>
+      <c r="D216" s="0">
+        <v>0.00024583944851884232</v>
+      </c>
+      <c r="E216" s="0">
+        <v>0.00016558538425519794</v>
+      </c>
+      <c r="F216" s="0">
+        <v>0.00013085054366301249</v>
+      </c>
+      <c r="G216" s="0">
+        <v>1.5168913096303569e-05</v>
+      </c>
+      <c r="H216" s="0">
+        <v>21.600000000000001</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="0">
+        <v>0.00038635419994989138</v>
+      </c>
+      <c r="B217" s="0">
+        <v>0.0003690735522066414</v>
+      </c>
+      <c r="C217" s="0">
+        <v>0.00033218613670190874</v>
+      </c>
+      <c r="D217" s="0">
+        <v>0.0002600973316340633</v>
+      </c>
+      <c r="E217" s="0">
+        <v>0.0001676841002176234</v>
+      </c>
+      <c r="F217" s="0">
+        <v>0.00014422095733116416</v>
+      </c>
+      <c r="G217" s="0">
+        <v>1.9473161581188467e-05</v>
+      </c>
+      <c r="H217" s="0">
+        <v>21.699999999999999</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="0">
+        <v>0.00042570267560940335</v>
+      </c>
+      <c r="B218" s="0">
+        <v>0.00038497430027418052</v>
+      </c>
+      <c r="C218" s="0">
+        <v>0.00028249763809656424</v>
+      </c>
+      <c r="D218" s="0">
+        <v>0.00025600024462552582</v>
+      </c>
+      <c r="E218" s="0">
+        <v>0.00016021270751400584</v>
+      </c>
+      <c r="F218" s="0">
+        <v>0.00013980811335005265</v>
+      </c>
+      <c r="G218" s="0">
+        <v>2.1558839395057611e-05</v>
+      </c>
+      <c r="H218" s="0">
+        <v>21.800000000000001</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="0">
+        <v>0.00039023478888633022</v>
+      </c>
+      <c r="B219" s="0">
+        <v>0.00038020383533981958</v>
+      </c>
+      <c r="C219" s="0">
+        <v>0.00035023304669740395</v>
+      </c>
+      <c r="D219" s="0">
+        <v>0.0002516478799932222</v>
+      </c>
+      <c r="E219" s="0">
+        <v>0.00017680605361869182</v>
+      </c>
+      <c r="F219" s="0">
+        <v>0.00012721930476823086</v>
+      </c>
+      <c r="G219" s="0">
+        <v>2.4767148855892695e-05</v>
+      </c>
+      <c r="H219" s="0">
+        <v>21.899999999999999</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="0">
         <v>0.00043438851066310768</v>
       </c>
-      <c r="B145" s="0">
+      <c r="B220" s="0">
         <v>0.00037374948608279586</v>
       </c>
-      <c r="C145" s="0">
+      <c r="C220" s="0">
         <v>0.00028423305165511438</v>
       </c>
-      <c r="D145" s="0">
+      <c r="D220" s="0">
         <v>0.00027266245976642612</v>
       </c>
-      <c r="E145" s="0">
+      <c r="E220" s="0">
         <v>0.00015750679474757048</v>
       </c>
-      <c r="F145" s="0">
+      <c r="F220" s="0">
         <v>0.00015188025604551437</v>
       </c>
-      <c r="G145" s="0">
+      <c r="G220" s="0">
         <v>2.8574713720893019e-05</v>
       </c>
-      <c r="H145" s="0">
+      <c r="H220" s="0">
         <v>22</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="0">
+        <v>0.00039563018313495924</v>
+      </c>
+      <c r="B221" s="0">
+        <v>0.00039300578144680303</v>
+      </c>
+      <c r="C221" s="0">
+        <v>0.00031904274055153818</v>
+      </c>
+      <c r="D221" s="0">
+        <v>0.00024597516585635719</v>
+      </c>
+      <c r="E221" s="0">
+        <v>0.0001897285022438576</v>
+      </c>
+      <c r="F221" s="0">
+        <v>0.00012080908713754127</v>
+      </c>
+      <c r="G221" s="0">
+        <v>3.0349919494558053e-05</v>
+      </c>
+      <c r="H221" s="0">
+        <v>22.100000000000001</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="0">
+        <v>0.00044399821278226791</v>
+      </c>
+      <c r="B222" s="0">
+        <v>0.00036408201603367249</v>
+      </c>
+      <c r="C222" s="0">
+        <v>0.00028772453134604794</v>
+      </c>
+      <c r="D222" s="0">
+        <v>0.00030736000000000001</v>
+      </c>
+      <c r="E222" s="0">
+        <v>0.00015763782029343755</v>
+      </c>
+      <c r="F222" s="0">
+        <v>0.00013913111491384967</v>
+      </c>
+      <c r="G222" s="0">
+        <v>3.5549461258301629e-05</v>
+      </c>
+      <c r="H222" s="0">
+        <v>22.199999999999999</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="0">
+        <v>0.00040120919874690416</v>
+      </c>
+      <c r="B223" s="0">
+        <v>0.0004246282673682491</v>
+      </c>
+      <c r="C223" s="0">
+        <v>0.0003004415999510046</v>
+      </c>
+      <c r="D223" s="0">
+        <v>0.0002423101621753526</v>
+      </c>
+      <c r="E223" s="0">
+        <v>0.00019898011401785359</v>
+      </c>
+      <c r="F223" s="0">
+        <v>0.00012049527574761195</v>
+      </c>
+      <c r="G223" s="0">
+        <v>3.8675776424983692e-05</v>
+      </c>
+      <c r="H223" s="0">
+        <v>22.300000000000001</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="0">
+        <v>0.0003807297763498329</v>
+      </c>
+      <c r="B224" s="0">
+        <v>0.00035009942635159393</v>
+      </c>
+      <c r="C224" s="0">
+        <v>0.00029221048072096797</v>
+      </c>
+      <c r="D224" s="0">
+        <v>0.00028800365117703281</v>
+      </c>
+      <c r="E224" s="0">
+        <v>0.00015735182160304137</v>
+      </c>
+      <c r="F224" s="0">
+        <v>0.00012200040081786708</v>
+      </c>
+      <c r="G224" s="0">
+        <v>4.1918788418056916e-05</v>
+      </c>
+      <c r="H224" s="0">
+        <v>22.399999999999999</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="0">
+        <v>0.00040731052495793566</v>
+      </c>
+      <c r="B225" s="0">
+        <v>0.00042448010705769428</v>
+      </c>
+      <c r="C225" s="0">
+        <v>0.00028994585513403677</v>
+      </c>
+      <c r="D225" s="0">
+        <v>0.00024125735542102506</v>
+      </c>
+      <c r="E225" s="0">
+        <v>0.00017879682588746855</v>
+      </c>
+      <c r="F225" s="0">
+        <v>0.0001228666879060725</v>
+      </c>
+      <c r="G225" s="0">
+        <v>4.0909101365367025e-05</v>
+      </c>
+      <c r="H225" s="0">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="0">
+        <v>0.00038272283283530479</v>
+      </c>
+      <c r="B226" s="0">
+        <v>0.00035797995295980256</v>
+      </c>
+      <c r="C226" s="0">
+        <v>0.00030490335424634963</v>
+      </c>
+      <c r="D226" s="0">
+        <v>0.00027376201516320428</v>
+      </c>
+      <c r="E226" s="0">
+        <v>0.00016022226137893964</v>
+      </c>
+      <c r="F226" s="0">
+        <v>0.00013052308964716256</v>
+      </c>
+      <c r="G226" s="0">
+        <v>4.1630319991382607e-05</v>
+      </c>
+      <c r="H226" s="0">
+        <v>22.600000000000001</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="0">
+        <v>0.0004140688786107283</v>
+      </c>
+      <c r="B227" s="0">
+        <v>0.00042432631199512525</v>
+      </c>
+      <c r="C227" s="0">
+        <v>0.00028450086476972445</v>
+      </c>
+      <c r="D227" s="0">
+        <v>0.00024314455457296108</v>
+      </c>
+      <c r="E227" s="0">
+        <v>0.00016924820544358542</v>
+      </c>
+      <c r="F227" s="0">
+        <v>0.00012807918688788344</v>
+      </c>
+      <c r="G227" s="0">
+        <v>3.9839705498829376e-05</v>
+      </c>
+      <c r="H227" s="0">
+        <v>22.699999999999999</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="0">
+        <v>0.00038563995727434151</v>
+      </c>
+      <c r="B228" s="0">
+        <v>0.00036691226683962836</v>
+      </c>
+      <c r="C228" s="0">
+        <v>0.00032599887335989252</v>
+      </c>
+      <c r="D228" s="0">
+        <v>0.00026249206891519258</v>
+      </c>
+      <c r="E228" s="0">
+        <v>0.00016579697239364646</v>
+      </c>
+      <c r="F228" s="0">
+        <v>0.00015223999999999999</v>
+      </c>
+      <c r="G228" s="0">
+        <v>4.1974309295379024e-05</v>
+      </c>
+      <c r="H228" s="0">
+        <v>22.800000000000001</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="0">
+        <v>0.00042129602197125342</v>
+      </c>
+      <c r="B229" s="0">
+        <v>0.0003916016480949231</v>
+      </c>
+      <c r="C229" s="0">
+        <v>0.00028243375826973298</v>
+      </c>
+      <c r="D229" s="0">
+        <v>0.00024996206470041229</v>
+      </c>
+      <c r="E229" s="0">
+        <v>0.00016260988088410869</v>
+      </c>
+      <c r="F229" s="0">
+        <v>0.00013551877498880818</v>
+      </c>
+      <c r="G229" s="0">
+        <v>4.1256284476019868e-05</v>
+      </c>
+      <c r="H229" s="0">
+        <v>22.899999999999999</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="0">
+        <v>0.00038916139073258464</v>
+      </c>
+      <c r="B230" s="0">
+        <v>0.00037720170969125571</v>
+      </c>
+      <c r="C230" s="0">
+        <v>0.00036125000000000003</v>
+      </c>
+      <c r="D230" s="0">
+        <v>0.00025353826483287371</v>
+      </c>
+      <c r="E230" s="0">
+        <v>0.00017414651951561466</v>
+      </c>
+      <c r="F230" s="0">
+        <v>0.00013059806770813204</v>
+      </c>
+      <c r="G230" s="0">
+        <v>4.2509171861215874e-05</v>
+      </c>
+      <c r="H230" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="0">
+        <v>0.00042923588667904906</v>
+      </c>
+      <c r="B231" s="0">
+        <v>0.00037988827821140215</v>
+      </c>
+      <c r="C231" s="0">
+        <v>0.00028292952224095075</v>
+      </c>
+      <c r="D231" s="0">
+        <v>0.00026199853053097575</v>
+      </c>
+      <c r="E231" s="0">
+        <v>0.00015895374443236499</v>
+      </c>
+      <c r="F231" s="0">
+        <v>0.00014530881159125674</v>
+      </c>
+      <c r="G231" s="0">
+        <v>4.3728686586382453e-05</v>
+      </c>
+      <c r="H231" s="0">
+        <v>23.100000000000001</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="0">
+        <v>0.00039399046477831164</v>
+      </c>
+      <c r="B232" s="0">
+        <v>0.00038895786228207956</v>
+      </c>
+      <c r="C232" s="0">
+        <v>0.00032679990113709394</v>
+      </c>
+      <c r="D232" s="0">
+        <v>0.00024722481727419178</v>
+      </c>
+      <c r="E232" s="0">
+        <v>0.00018458668177698912</v>
+      </c>
+      <c r="F232" s="0">
+        <v>0.0001224659745971135</v>
+      </c>
+      <c r="G232" s="0">
+        <v>4.4243774415481011e-05</v>
+      </c>
+      <c r="H232" s="0">
+        <v>23.199999999999999</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="0">
+        <v>0.00043776662703434287</v>
+      </c>
+      <c r="B233" s="0">
+        <v>0.00036995807920001188</v>
+      </c>
+      <c r="C233" s="0">
+        <v>0.00028528202912184842</v>
+      </c>
+      <c r="D233" s="0">
+        <v>0.0002831436363629579</v>
+      </c>
+      <c r="E233" s="0">
+        <v>0.00015713988541037353</v>
+      </c>
+      <c r="F233" s="0">
+        <v>0.00015226241802971218</v>
+      </c>
+      <c r="G233" s="0">
+        <v>4.7176815894116879e-05</v>
+      </c>
+      <c r="H233" s="0">
+        <v>23.300000000000001</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="0">
+        <v>0.00039909061214534066</v>
+      </c>
+      <c r="B234" s="0">
+        <v>0.00040265339383000967</v>
+      </c>
+      <c r="C234" s="0">
+        <v>0.00030580042175913495</v>
+      </c>
+      <c r="D234" s="0">
+        <v>0.00024336645384048631</v>
+      </c>
+      <c r="E234" s="0">
+        <v>0.00019914063562046137</v>
+      </c>
+      <c r="F234" s="0">
+        <v>0.00012061462803552645</v>
+      </c>
+      <c r="G234" s="0">
+        <v>4.8588392787039855e-05</v>
+      </c>
+      <c r="H234" s="0">
+        <v>23.399999999999999</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="0">
+        <v>0.00038050451941732939</v>
+      </c>
+      <c r="B235" s="0">
+        <v>0.00034933944392870098</v>
+      </c>
+      <c r="C235" s="0">
+        <v>0.00029135616875569387</v>
+      </c>
+      <c r="D235" s="0">
+        <v>0.00028993736139816507</v>
+      </c>
+      <c r="E235" s="0">
+        <v>0.00015713665595153446</v>
+      </c>
+      <c r="F235" s="0">
+        <v>0.00012205842215102155</v>
+      </c>
+      <c r="G235" s="0">
+        <v>5.6084231619923755e-05</v>
+      </c>
+      <c r="H235" s="0">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="0">
+        <v>0.00040474314669137806</v>
+      </c>
+      <c r="B236" s="0">
+        <v>0.00042446834862294307</v>
+      </c>
+      <c r="C236" s="0">
+        <v>0.00029329496143591589</v>
+      </c>
+      <c r="D236" s="0">
+        <v>0.00024127253556047569</v>
+      </c>
+      <c r="E236" s="0">
+        <v>0.00018329334331838309</v>
+      </c>
+      <c r="F236" s="0">
+        <v>0.00012209469312596027</v>
+      </c>
+      <c r="G236" s="0">
+        <v>5.4018277091495585e-05</v>
+      </c>
+      <c r="H236" s="0">
+        <v>23.600000000000001</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="0">
+        <v>0.00038233569055727199</v>
+      </c>
+      <c r="B237" s="0">
+        <v>0.00035673772384881469</v>
+      </c>
+      <c r="C237" s="0">
+        <v>0.00030247082610025363</v>
+      </c>
+      <c r="D237" s="0">
+        <v>0.00027532655397575616</v>
+      </c>
+      <c r="E237" s="0">
+        <v>0.00015961679476413364</v>
+      </c>
+      <c r="F237" s="0">
+        <v>0.0001288234238075822</v>
+      </c>
+      <c r="G237" s="0">
+        <v>5.0325652268918047e-05</v>
+      </c>
+      <c r="H237" s="0">
+        <v>23.699999999999999</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="0">
+        <v>0.00041084810547048316</v>
+      </c>
+      <c r="B238" s="0">
+        <v>0.0004243159354243765</v>
+      </c>
+      <c r="C238" s="0">
+        <v>0.00028637459369051899</v>
+      </c>
+      <c r="D238" s="0">
+        <v>0.00024192552483831323</v>
+      </c>
+      <c r="E238" s="0">
+        <v>0.00017321072176649968</v>
+      </c>
+      <c r="F238" s="0">
+        <v>0.00012599909294141792</v>
+      </c>
+      <c r="G238" s="0">
+        <v>4.8136822493230033e-05</v>
+      </c>
+      <c r="H238" s="0">
+        <v>23.800000000000001</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="0">
+        <v>0.00038535829890100088</v>
+      </c>
+      <c r="B239" s="0">
+        <v>0.00036550078054167643</v>
+      </c>
+      <c r="C239" s="0">
+        <v>0.00032154270685602604</v>
+      </c>
+      <c r="D239" s="0">
+        <v>0.00026400791982415713</v>
+      </c>
+      <c r="E239" s="0">
+        <v>0.00016472750502485094</v>
+      </c>
+      <c r="F239" s="0">
+        <v>0.00014728375900364623</v>
+      </c>
+      <c r="G239" s="0">
+        <v>4.6888216001813104e-05</v>
+      </c>
+      <c r="H239" s="0">
+        <v>23.899999999999999</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="0">
+        <v>0.00041857982080873942</v>
+      </c>
+      <c r="B240" s="0">
+        <v>0.00039911171629076813</v>
+      </c>
+      <c r="C240" s="0">
+        <v>0.0002838010722661395</v>
+      </c>
+      <c r="D240" s="0">
+        <v>0.00024646070455972328</v>
+      </c>
+      <c r="E240" s="0">
+        <v>0.00016635052894112306</v>
+      </c>
+      <c r="F240" s="0">
+        <v>0.0001322783500528302</v>
+      </c>
+      <c r="G240" s="0">
+        <v>4.7677550146622917e-05</v>
+      </c>
+      <c r="H240" s="0">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>